<commit_message>
Reseatchin someones AIS generator
</commit_message>
<xml_diff>
--- a/test_bl/resources/tests/TrassaTests_v01.xlsx
+++ b/test_bl/resources/tests/TrassaTests_v01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13380"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13380" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="trassa_Tests" sheetId="3" r:id="rId1"/>
@@ -1500,7 +1500,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1555,8 +1555,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1570,15 +1568,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1592,9 +1581,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1683,6 +1669,26 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -2088,7 +2094,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -2106,290 +2112,290 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="54" t="s">
         <v>327</v>
       </c>
-      <c r="C2" s="60" t="s">
+      <c r="C2" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="61" t="s">
+      <c r="D2" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="60" t="s">
+      <c r="E2" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="60" t="s">
+      <c r="F2" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="60" t="s">
+      <c r="G2" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="60" t="s">
+      <c r="H2" s="54" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="37">
+      <c r="A3" s="31">
         <v>1</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="31" t="s">
         <v>333</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="32" t="s">
         <v>335</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="31" t="s">
         <v>329</v>
       </c>
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="33" t="s">
         <v>330</v>
       </c>
-      <c r="F3" s="39" t="s">
+      <c r="F3" s="33" t="s">
         <v>340</v>
       </c>
-      <c r="G3" s="39"/>
-      <c r="H3" s="40"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="34"/>
     </row>
     <row r="4" spans="1:8" ht="87" x14ac:dyDescent="0.35">
-      <c r="A4" s="37">
+      <c r="A4" s="31">
         <v>2</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="31" t="s">
         <v>333</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="32" t="s">
         <v>336</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="31" t="s">
         <v>328</v>
       </c>
-      <c r="E4" s="39" t="s">
+      <c r="E4" s="33" t="s">
         <v>331</v>
       </c>
-      <c r="F4" s="39" t="s">
+      <c r="F4" s="33" t="s">
         <v>339</v>
       </c>
-      <c r="G4" s="39"/>
-      <c r="H4" s="40"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="34"/>
     </row>
     <row r="5" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A5" s="37">
+      <c r="A5" s="31">
         <v>3</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="31" t="s">
         <v>333</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="32" t="s">
         <v>369</v>
       </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="39" t="s">
+      <c r="D5" s="31"/>
+      <c r="E5" s="33" t="s">
         <v>370</v>
       </c>
-      <c r="F5" s="39" t="s">
+      <c r="F5" s="33" t="s">
         <v>371</v>
       </c>
-      <c r="G5" s="39"/>
-      <c r="H5" s="40"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="34"/>
     </row>
     <row r="6" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A6" s="37">
+      <c r="A6" s="31">
         <v>4</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="31" t="s">
         <v>333</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="32" t="s">
         <v>372</v>
       </c>
-      <c r="D6" s="37"/>
-      <c r="E6" s="39" t="s">
+      <c r="D6" s="31"/>
+      <c r="E6" s="33" t="s">
         <v>374</v>
       </c>
-      <c r="F6" s="39" t="s">
+      <c r="F6" s="33" t="s">
         <v>373</v>
       </c>
-      <c r="G6" s="39"/>
-      <c r="H6" s="40"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="34"/>
     </row>
     <row r="7" spans="1:8" ht="87" x14ac:dyDescent="0.35">
-      <c r="A7" s="37">
+      <c r="A7" s="31">
         <v>5</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="31" t="s">
         <v>333</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="32" t="s">
         <v>336</v>
       </c>
-      <c r="D7" s="37" t="s">
+      <c r="D7" s="31" t="s">
         <v>328</v>
       </c>
-      <c r="E7" s="39" t="s">
+      <c r="E7" s="33" t="s">
         <v>331</v>
       </c>
-      <c r="F7" s="39" t="s">
+      <c r="F7" s="33" t="s">
         <v>339</v>
       </c>
-      <c r="G7" s="39"/>
-      <c r="H7" s="40"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="34"/>
     </row>
     <row r="8" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="37">
+      <c r="A8" s="31">
         <v>6</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="31" t="s">
         <v>333</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="32" t="s">
         <v>332</v>
       </c>
-      <c r="D8" s="37"/>
-      <c r="E8" s="39" t="s">
+      <c r="D8" s="31"/>
+      <c r="E8" s="33" t="s">
         <v>367</v>
       </c>
-      <c r="F8" s="39" t="s">
+      <c r="F8" s="33" t="s">
         <v>341</v>
       </c>
-      <c r="G8" s="39"/>
-      <c r="H8" s="40"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="34"/>
     </row>
     <row r="9" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A9" s="60">
+      <c r="A9" s="54">
         <v>7</v>
       </c>
-      <c r="B9" s="60" t="s">
+      <c r="B9" s="54" t="s">
         <v>334</v>
       </c>
-      <c r="C9" s="62" t="s">
+      <c r="C9" s="56" t="s">
         <v>337</v>
       </c>
-      <c r="D9" s="60"/>
-      <c r="E9" s="63" t="s">
+      <c r="D9" s="54"/>
+      <c r="E9" s="57" t="s">
         <v>338</v>
       </c>
-      <c r="F9" s="63" t="s">
+      <c r="F9" s="57" t="s">
         <v>342</v>
       </c>
-      <c r="G9" s="63"/>
-      <c r="H9" s="64"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="58"/>
     </row>
     <row r="10" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A10" s="60">
+      <c r="A10" s="54">
         <v>8</v>
       </c>
-      <c r="B10" s="60" t="s">
+      <c r="B10" s="54" t="s">
         <v>334</v>
       </c>
-      <c r="C10" s="62" t="s">
+      <c r="C10" s="56" t="s">
         <v>352</v>
       </c>
-      <c r="D10" s="60"/>
-      <c r="E10" s="63" t="s">
+      <c r="D10" s="54"/>
+      <c r="E10" s="57" t="s">
         <v>365</v>
       </c>
-      <c r="F10" s="63" t="s">
+      <c r="F10" s="57" t="s">
         <v>354</v>
       </c>
-      <c r="G10" s="63"/>
-      <c r="H10" s="64"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="58"/>
     </row>
     <row r="11" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="60">
+      <c r="A11" s="54">
         <v>9</v>
       </c>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="54" t="s">
         <v>334</v>
       </c>
-      <c r="C11" s="62" t="s">
+      <c r="C11" s="56" t="s">
         <v>353</v>
       </c>
-      <c r="D11" s="60"/>
-      <c r="E11" s="63" t="s">
+      <c r="D11" s="54"/>
+      <c r="E11" s="57" t="s">
         <v>366</v>
       </c>
-      <c r="F11" s="63" t="s">
+      <c r="F11" s="57" t="s">
         <v>362</v>
       </c>
-      <c r="G11" s="63"/>
-      <c r="H11" s="64"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="58"/>
     </row>
     <row r="12" spans="1:8" ht="58" x14ac:dyDescent="0.35">
-      <c r="A12" s="60">
+      <c r="A12" s="54">
         <v>10</v>
       </c>
-      <c r="B12" s="60" t="s">
+      <c r="B12" s="54" t="s">
         <v>334</v>
       </c>
-      <c r="C12" s="62" t="s">
+      <c r="C12" s="56" t="s">
         <v>363</v>
       </c>
-      <c r="D12" s="64"/>
-      <c r="E12" s="63" t="s">
+      <c r="D12" s="58"/>
+      <c r="E12" s="57" t="s">
         <v>368</v>
       </c>
-      <c r="F12" s="63" t="s">
+      <c r="F12" s="57" t="s">
         <v>375</v>
       </c>
-      <c r="G12" s="64"/>
-      <c r="H12" s="64"/>
+      <c r="G12" s="58"/>
+      <c r="H12" s="58"/>
     </row>
     <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="60">
+      <c r="A13" s="54">
         <v>11</v>
       </c>
-      <c r="B13" s="60" t="s">
+      <c r="B13" s="54" t="s">
         <v>334</v>
       </c>
-      <c r="C13" s="62"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="63" t="s">
+      <c r="C13" s="56"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="57" t="s">
         <v>368</v>
       </c>
-      <c r="F13" s="63" t="s">
+      <c r="F13" s="57" t="s">
         <v>376</v>
       </c>
-      <c r="G13" s="64"/>
-      <c r="H13" s="64"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="58"/>
     </row>
     <row r="14" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="60">
+      <c r="A14" s="54">
         <v>12</v>
       </c>
-      <c r="B14" s="60" t="s">
+      <c r="B14" s="54" t="s">
         <v>334</v>
       </c>
-      <c r="C14" s="62"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="63" t="s">
+      <c r="C14" s="56"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="57" t="s">
         <v>377</v>
       </c>
-      <c r="F14" s="63" t="s">
+      <c r="F14" s="57" t="s">
         <v>375</v>
       </c>
-      <c r="G14" s="64"/>
-      <c r="H14" s="64"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="58"/>
     </row>
     <row r="15" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="60">
+      <c r="A15" s="54">
         <v>13</v>
       </c>
-      <c r="B15" s="60" t="s">
+      <c r="B15" s="54" t="s">
         <v>334</v>
       </c>
-      <c r="C15" s="62"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="63" t="s">
+      <c r="C15" s="56"/>
+      <c r="D15" s="58"/>
+      <c r="E15" s="57" t="s">
         <v>377</v>
       </c>
-      <c r="F15" s="63" t="s">
+      <c r="F15" s="57" t="s">
         <v>376</v>
       </c>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
+      <c r="G15" s="58"/>
+      <c r="H15" s="58"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2708,19 +2714,19 @@
     <col min="5" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:4" s="43" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="46" t="s">
         <v>138</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="47" t="s">
         <v>346</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="43" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="44" t="s">
         <v>139</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -2731,7 +2737,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="44" t="s">
         <v>140</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -2742,7 +2748,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="45" t="s">
         <v>141</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -2753,7 +2759,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="44" t="s">
         <v>142</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -2764,7 +2770,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="44" t="s">
         <v>143</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -2775,7 +2781,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="50" t="s">
+      <c r="A7" s="44" t="s">
         <v>144</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -2789,7 +2795,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="50" t="s">
+      <c r="A8" s="44" t="s">
         <v>145</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -2800,7 +2806,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="50" t="s">
+      <c r="A9" s="44" t="s">
         <v>146</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -2811,7 +2817,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="44" t="s">
         <v>343</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -2822,7 +2828,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="50" t="s">
+      <c r="A11" s="44" t="s">
         <v>344</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -2844,63 +2850,63 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.90625" style="33" customWidth="1"/>
+    <col min="1" max="1" width="10.26953125" style="28" customWidth="1"/>
     <col min="2" max="2" width="8.7265625" style="3"/>
     <col min="3" max="3" width="23.6328125" style="3" customWidth="1"/>
     <col min="4" max="4" width="21" style="3" customWidth="1"/>
     <col min="5" max="5" width="8.7265625" style="3"/>
-    <col min="6" max="6" width="60.7265625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="44.81640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="8.7265625" style="3"/>
     <col min="8" max="8" width="10.6328125" style="3" customWidth="1"/>
     <col min="9" max="9" width="50.08984375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="55" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="65" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
     </row>
     <row r="2" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="59" t="s">
         <v>170</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="H2" s="29" t="s">
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="H2" s="24" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="63" t="s">
         <v>54</v>
       </c>
       <c r="H3" s="18">
@@ -2911,7 +2917,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="26" t="s">
         <v>55</v>
       </c>
       <c r="B4" s="18">
@@ -2926,7 +2932,7 @@
       <c r="E4" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="64" t="s">
         <v>173</v>
       </c>
       <c r="H4" s="18">
@@ -2937,7 +2943,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="31">
+      <c r="A5" s="26">
         <v>43287</v>
       </c>
       <c r="B5" s="18">
@@ -2952,7 +2958,7 @@
       <c r="E5" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="64" t="s">
         <v>175</v>
       </c>
       <c r="H5" s="18">
@@ -2963,7 +2969,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="31">
+      <c r="A6" s="26">
         <v>13728</v>
       </c>
       <c r="B6" s="18">
@@ -2978,7 +2984,7 @@
       <c r="E6" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="64" t="s">
         <v>67</v>
       </c>
       <c r="H6" s="18">
@@ -2989,7 +2995,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="26" t="s">
         <v>178</v>
       </c>
       <c r="B7" s="18">
@@ -3004,7 +3010,7 @@
       <c r="E7" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="64" t="s">
         <v>182</v>
       </c>
       <c r="H7" s="18">
@@ -3015,7 +3021,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="26" t="s">
         <v>184</v>
       </c>
       <c r="B8" s="18">
@@ -3030,7 +3036,7 @@
       <c r="E8" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="64" t="s">
         <v>81</v>
       </c>
       <c r="H8" s="18">
@@ -3041,7 +3047,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="26" t="s">
         <v>189</v>
       </c>
       <c r="B9" s="18">
@@ -3056,7 +3062,7 @@
       <c r="E9" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="64" t="s">
         <v>81</v>
       </c>
       <c r="H9" s="18">
@@ -3067,7 +3073,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="26" t="s">
         <v>192</v>
       </c>
       <c r="B10" s="18">
@@ -3082,7 +3088,7 @@
       <c r="E10" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="64" t="s">
         <v>81</v>
       </c>
       <c r="H10" s="18">
@@ -3093,7 +3099,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="26" t="s">
         <v>194</v>
       </c>
       <c r="B11" s="18">
@@ -3108,7 +3114,7 @@
       <c r="E11" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="64" t="s">
         <v>195</v>
       </c>
       <c r="H11" s="18">
@@ -3119,7 +3125,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="26" t="s">
         <v>197</v>
       </c>
       <c r="B12" s="18">
@@ -3134,7 +3140,7 @@
       <c r="E12" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="64" t="s">
         <v>195</v>
       </c>
       <c r="H12" s="18">
@@ -3145,7 +3151,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="26" t="s">
         <v>199</v>
       </c>
       <c r="B13" s="18">
@@ -3160,7 +3166,7 @@
       <c r="E13" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="64" t="s">
         <v>201</v>
       </c>
       <c r="H13" s="18">
@@ -3171,7 +3177,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="26" t="s">
         <v>203</v>
       </c>
       <c r="B14" s="18">
@@ -3186,7 +3192,7 @@
       <c r="E14" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="F14" s="64" t="s">
         <v>205</v>
       </c>
       <c r="H14" s="18">
@@ -3197,7 +3203,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="26" t="s">
         <v>207</v>
       </c>
       <c r="B15" s="18">
@@ -3212,7 +3218,7 @@
       <c r="E15" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="64" t="s">
         <v>208</v>
       </c>
       <c r="H15" s="18">
@@ -3223,7 +3229,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="26" t="s">
         <v>209</v>
       </c>
       <c r="B16" s="18">
@@ -3238,7 +3244,7 @@
       <c r="E16" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="F16" s="64" t="s">
         <v>212</v>
       </c>
       <c r="H16" s="18">
@@ -3249,7 +3255,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="26" t="s">
         <v>213</v>
       </c>
       <c r="B17" s="18">
@@ -3258,11 +3264,11 @@
       <c r="C17" s="18" t="s">
         <v>214</v>
       </c>
-      <c r="D17" s="32"/>
+      <c r="D17" s="27"/>
       <c r="E17" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="F17" s="18" t="s">
+      <c r="F17" s="64" t="s">
         <v>72</v>
       </c>
       <c r="H17" s="18">
@@ -3273,7 +3279,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="26" t="s">
         <v>216</v>
       </c>
       <c r="B18" s="18">
@@ -3288,7 +3294,7 @@
       <c r="E18" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="F18" s="18" t="s">
+      <c r="F18" s="64" t="s">
         <v>81</v>
       </c>
       <c r="H18" s="18">
@@ -3299,7 +3305,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="26" t="s">
         <v>218</v>
       </c>
       <c r="B19" s="18">
@@ -3314,7 +3320,7 @@
       <c r="E19" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="F19" s="18" t="s">
+      <c r="F19" s="64" t="s">
         <v>81</v>
       </c>
     </row>
@@ -3338,48 +3344,48 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.36328125" style="25" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" style="25"/>
-    <col min="3" max="3" width="28.1796875" style="25" customWidth="1"/>
-    <col min="4" max="5" width="8.7265625" style="25"/>
-    <col min="6" max="6" width="54.1796875" style="25" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="21"/>
+    <col min="1" max="1" width="26.36328125" style="23" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" style="23"/>
+    <col min="3" max="3" width="28.1796875" style="23" customWidth="1"/>
+    <col min="4" max="5" width="8.7265625" style="23"/>
+    <col min="6" max="6" width="54.1796875" style="23" customWidth="1"/>
+    <col min="7" max="16384" width="8.7265625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
     </row>
     <row r="2" spans="1:13" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="20" t="s">
         <v>54</v>
       </c>
     </row>
@@ -3404,7 +3410,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="21" t="s">
         <v>60</v>
       </c>
       <c r="B4" s="18">
@@ -3424,7 +3430,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="21" t="s">
         <v>64</v>
       </c>
       <c r="B5" s="18">
@@ -3779,7 +3785,7 @@
       <c r="E22" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="F22" s="24" t="s">
+      <c r="F22" s="22" t="s">
         <v>137</v>
       </c>
     </row>
@@ -3804,7 +3810,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="54"/>
+    <col min="1" max="1" width="8.7265625" style="48"/>
     <col min="2" max="2" width="17.90625" style="4" customWidth="1"/>
     <col min="3" max="3" width="22.1796875" style="4" customWidth="1"/>
     <col min="4" max="4" width="21.453125" style="4" customWidth="1"/>
@@ -3813,79 +3819,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="51" t="s">
         <v>157</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="35" t="s">
+      <c r="B1" s="50"/>
+      <c r="C1" s="29" t="s">
         <v>355</v>
       </c>
-      <c r="D1" s="59" t="s">
+      <c r="D1" s="53" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="49" t="s">
         <v>158</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="50" t="s">
         <v>164</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="30" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="49" t="s">
         <v>159</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="50" t="s">
         <v>165</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="30" t="s">
         <v>358</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="52" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="49" t="s">
         <v>160</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="50" t="s">
         <v>166</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="30" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="55" t="s">
+      <c r="A5" s="49" t="s">
         <v>161</v>
       </c>
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="50" t="s">
         <v>167</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="30" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="49" t="s">
         <v>162</v>
       </c>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="50" t="s">
         <v>168</v>
       </c>
-      <c r="C6" s="36"/>
+      <c r="C6" s="30"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="49" t="s">
         <v>163</v>
       </c>
-      <c r="B7" s="56"/>
-      <c r="C7" s="36"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3903,790 +3909,790 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.7265625" style="25" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" style="25"/>
-    <col min="3" max="3" width="27.36328125" style="25" customWidth="1"/>
-    <col min="4" max="4" width="18.54296875" style="25" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" style="25"/>
-    <col min="6" max="6" width="32.81640625" style="25" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" style="41"/>
-    <col min="8" max="8" width="13.26953125" style="41" customWidth="1"/>
-    <col min="9" max="9" width="8.7265625" style="41"/>
-    <col min="10" max="10" width="37.1796875" style="41" customWidth="1"/>
-    <col min="11" max="11" width="33.90625" style="41" customWidth="1"/>
-    <col min="12" max="12" width="8.7265625" style="41"/>
-    <col min="13" max="13" width="64.54296875" style="41" customWidth="1"/>
-    <col min="14" max="16384" width="8.7265625" style="41"/>
+    <col min="1" max="1" width="19.7265625" style="23" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" style="23"/>
+    <col min="3" max="3" width="27.36328125" style="23" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" style="23" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="23"/>
+    <col min="6" max="6" width="32.81640625" style="23" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" style="35"/>
+    <col min="8" max="8" width="13.26953125" style="35" customWidth="1"/>
+    <col min="9" max="9" width="8.7265625" style="35"/>
+    <col min="10" max="10" width="37.1796875" style="35" customWidth="1"/>
+    <col min="11" max="11" width="33.90625" style="35" customWidth="1"/>
+    <col min="12" max="12" width="8.7265625" style="35"/>
+    <col min="13" max="13" width="64.54296875" style="35" customWidth="1"/>
+    <col min="14" max="16384" width="8.7265625" style="35"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="23" t="s">
         <v>291</v>
       </c>
-      <c r="H1" s="47" t="s">
+      <c r="H1" s="41" t="s">
         <v>219</v>
       </c>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
     </row>
     <row r="2" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="42" t="s">
+      <c r="E2" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="42" t="s">
+      <c r="F2" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="42" t="s">
+      <c r="H2" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="I2" s="42" t="s">
+      <c r="I2" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="J2" s="42" t="s">
+      <c r="J2" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="K2" s="42" t="s">
+      <c r="K2" s="36" t="s">
         <v>220</v>
       </c>
-      <c r="L2" s="42" t="s">
+      <c r="L2" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="M2" s="42" t="s">
+      <c r="M2" s="36" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="43">
+      <c r="B3" s="37">
         <v>6</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="D3" s="43" t="s">
+      <c r="D3" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="E3" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="37" t="s">
         <v>292</v>
       </c>
-      <c r="H3" s="43" t="s">
+      <c r="H3" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="I3" s="43">
+      <c r="I3" s="37">
         <v>6</v>
       </c>
-      <c r="J3" s="43" t="s">
+      <c r="J3" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="K3" s="43" t="s">
+      <c r="K3" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="L3" s="43" t="s">
+      <c r="L3" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="M3" s="43" t="s">
+      <c r="M3" s="37" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="43">
+      <c r="B4" s="37">
         <v>2</v>
       </c>
-      <c r="C4" s="43" t="s">
+      <c r="C4" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="43" t="s">
+      <c r="D4" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="43" t="s">
+      <c r="E4" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="43" t="s">
+      <c r="F4" s="37" t="s">
         <v>293</v>
       </c>
-      <c r="H4" s="44" t="s">
+      <c r="H4" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="I4" s="43">
+      <c r="I4" s="37">
         <v>2</v>
       </c>
-      <c r="J4" s="43" t="s">
+      <c r="J4" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="K4" s="43" t="s">
+      <c r="K4" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="L4" s="43" t="s">
+      <c r="L4" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="M4" s="43" t="s">
+      <c r="M4" s="37" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="43">
+      <c r="B5" s="37">
         <v>30</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="43" t="s">
+      <c r="D5" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="E5" s="43" t="s">
+      <c r="E5" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="43" t="s">
+      <c r="F5" s="37" t="s">
         <v>223</v>
       </c>
-      <c r="H5" s="44" t="s">
+      <c r="H5" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="I5" s="43">
+      <c r="I5" s="37">
         <v>30</v>
       </c>
-      <c r="J5" s="48" t="s">
+      <c r="J5" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="K5" s="43" t="s">
+      <c r="K5" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="L5" s="43" t="s">
+      <c r="L5" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="M5" s="43" t="s">
+      <c r="M5" s="37" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="37" t="s">
         <v>224</v>
       </c>
-      <c r="B6" s="43">
+      <c r="B6" s="37">
         <v>2</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="C6" s="37" t="s">
         <v>294</v>
       </c>
-      <c r="D6" s="43" t="s">
+      <c r="D6" s="37" t="s">
         <v>295</v>
       </c>
-      <c r="E6" s="43" t="s">
+      <c r="E6" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="43" t="s">
+      <c r="F6" s="37" t="s">
         <v>296</v>
       </c>
-      <c r="H6" s="43" t="s">
+      <c r="H6" s="37" t="s">
         <v>224</v>
       </c>
-      <c r="I6" s="43">
+      <c r="I6" s="37">
         <v>2</v>
       </c>
-      <c r="J6" s="43" t="s">
+      <c r="J6" s="37" t="s">
         <v>225</v>
       </c>
-      <c r="K6" s="43" t="s">
+      <c r="K6" s="37" t="s">
         <v>226</v>
       </c>
-      <c r="L6" s="43" t="s">
+      <c r="L6" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="M6" s="45" t="s">
+      <c r="M6" s="39" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="37" t="s">
         <v>297</v>
       </c>
-      <c r="B7" s="43">
+      <c r="B7" s="37">
         <v>120</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="42" t="s">
         <v>238</v>
       </c>
-      <c r="D7" s="43" t="s">
+      <c r="D7" s="37" t="s">
         <v>239</v>
       </c>
-      <c r="E7" s="43" t="s">
+      <c r="E7" s="37" t="s">
         <v>235</v>
       </c>
-      <c r="F7" s="43" t="s">
+      <c r="F7" s="37" t="s">
         <v>298</v>
       </c>
-      <c r="H7" s="43" t="s">
+      <c r="H7" s="37" t="s">
         <v>228</v>
       </c>
-      <c r="I7" s="43">
+      <c r="I7" s="37">
         <v>30</v>
       </c>
-      <c r="J7" s="48" t="s">
+      <c r="J7" s="42" t="s">
         <v>229</v>
       </c>
-      <c r="K7" s="43" t="s">
+      <c r="K7" s="37" t="s">
         <v>230</v>
       </c>
-      <c r="L7" s="43" t="s">
+      <c r="L7" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="M7" s="43" t="s">
+      <c r="M7" s="37" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="37" t="s">
         <v>299</v>
       </c>
-      <c r="B8" s="43">
+      <c r="B8" s="37">
         <v>8</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="D8" s="46"/>
-      <c r="E8" s="43" t="s">
+      <c r="D8" s="40"/>
+      <c r="E8" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="F8" s="43" t="s">
+      <c r="F8" s="37" t="s">
         <v>300</v>
       </c>
-      <c r="H8" s="43" t="s">
+      <c r="H8" s="37" t="s">
         <v>232</v>
       </c>
-      <c r="I8" s="43">
+      <c r="I8" s="37">
         <v>42</v>
       </c>
-      <c r="J8" s="48" t="s">
+      <c r="J8" s="42" t="s">
         <v>233</v>
       </c>
-      <c r="K8" s="43" t="s">
+      <c r="K8" s="37" t="s">
         <v>234</v>
       </c>
-      <c r="L8" s="43" t="s">
+      <c r="L8" s="37" t="s">
         <v>235</v>
       </c>
-      <c r="M8" s="43" t="s">
+      <c r="M8" s="37" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="37" t="s">
         <v>301</v>
       </c>
-      <c r="B9" s="43">
+      <c r="B9" s="37">
         <v>8</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="37" t="s">
         <v>242</v>
       </c>
-      <c r="D9" s="43" t="s">
+      <c r="D9" s="37" t="s">
         <v>243</v>
       </c>
-      <c r="E9" s="43" t="s">
+      <c r="E9" s="37" t="s">
         <v>181</v>
       </c>
-      <c r="F9" s="43" t="s">
+      <c r="F9" s="37" t="s">
         <v>302</v>
       </c>
-      <c r="H9" s="43" t="s">
+      <c r="H9" s="37" t="s">
         <v>237</v>
       </c>
-      <c r="I9" s="43">
+      <c r="I9" s="37">
         <v>120</v>
       </c>
-      <c r="J9" s="43" t="s">
+      <c r="J9" s="37" t="s">
         <v>238</v>
       </c>
-      <c r="K9" s="43" t="s">
+      <c r="K9" s="37" t="s">
         <v>239</v>
       </c>
-      <c r="L9" s="43" t="s">
+      <c r="L9" s="37" t="s">
         <v>235</v>
       </c>
-      <c r="M9" s="43" t="s">
+      <c r="M9" s="37" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="37" t="s">
         <v>303</v>
       </c>
-      <c r="B10" s="43">
+      <c r="B10" s="37">
         <v>18</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="37" t="s">
         <v>304</v>
       </c>
-      <c r="D10" s="43" t="s">
+      <c r="D10" s="37" t="s">
         <v>305</v>
       </c>
-      <c r="E10" s="43" t="s">
+      <c r="E10" s="37" t="s">
         <v>235</v>
       </c>
-      <c r="F10" s="43" t="s">
+      <c r="F10" s="37" t="s">
         <v>306</v>
       </c>
-      <c r="H10" s="43" t="s">
+      <c r="H10" s="37" t="s">
         <v>241</v>
       </c>
-      <c r="I10" s="43">
+      <c r="I10" s="37">
         <v>8</v>
       </c>
-      <c r="J10" s="43" t="s">
+      <c r="J10" s="37" t="s">
         <v>242</v>
       </c>
-      <c r="K10" s="43" t="s">
+      <c r="K10" s="37" t="s">
         <v>243</v>
       </c>
-      <c r="L10" s="43" t="s">
+      <c r="L10" s="37" t="s">
         <v>181</v>
       </c>
-      <c r="M10" s="43" t="s">
+      <c r="M10" s="37" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="43" t="s">
+      <c r="A11" s="37" t="s">
         <v>307</v>
       </c>
-      <c r="B11" s="43">
+      <c r="B11" s="37">
         <v>4</v>
       </c>
-      <c r="C11" s="43" t="s">
+      <c r="C11" s="37" t="s">
         <v>308</v>
       </c>
-      <c r="D11" s="43" t="s">
+      <c r="D11" s="37" t="s">
         <v>309</v>
       </c>
-      <c r="E11" s="43" t="s">
+      <c r="E11" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="43" t="s">
+      <c r="F11" s="37" t="s">
         <v>310</v>
       </c>
-      <c r="H11" s="43" t="s">
+      <c r="H11" s="37" t="s">
         <v>245</v>
       </c>
-      <c r="I11" s="43">
+      <c r="I11" s="37">
         <v>9</v>
       </c>
-      <c r="J11" s="43" t="s">
+      <c r="J11" s="37" t="s">
         <v>246</v>
       </c>
-      <c r="K11" s="43" t="s">
+      <c r="K11" s="37" t="s">
         <v>247</v>
       </c>
-      <c r="L11" s="43" t="s">
+      <c r="L11" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="M11" s="43" t="s">
+      <c r="M11" s="37" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="37" t="s">
         <v>311</v>
       </c>
-      <c r="B12" s="43">
+      <c r="B12" s="37">
         <v>20</v>
       </c>
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="37" t="s">
         <v>312</v>
       </c>
-      <c r="D12" s="43" t="s">
+      <c r="D12" s="37" t="s">
         <v>313</v>
       </c>
-      <c r="E12" s="43" t="s">
+      <c r="E12" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="43" t="s">
+      <c r="F12" s="37" t="s">
         <v>310</v>
       </c>
-      <c r="H12" s="43" t="s">
+      <c r="H12" s="37" t="s">
         <v>249</v>
       </c>
-      <c r="I12" s="43">
+      <c r="I12" s="37">
         <v>9</v>
       </c>
-      <c r="J12" s="43" t="s">
+      <c r="J12" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="K12" s="43" t="s">
+      <c r="K12" s="37" t="s">
         <v>251</v>
       </c>
-      <c r="L12" s="43" t="s">
+      <c r="L12" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="M12" s="43" t="s">
+      <c r="M12" s="37" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="37" t="s">
         <v>314</v>
       </c>
-      <c r="B13" s="43">
+      <c r="B13" s="37">
         <v>42</v>
       </c>
-      <c r="C13" s="48" t="s">
+      <c r="C13" s="42" t="s">
         <v>233</v>
       </c>
-      <c r="D13" s="43" t="s">
+      <c r="D13" s="37" t="s">
         <v>234</v>
       </c>
-      <c r="E13" s="43" t="s">
+      <c r="E13" s="37" t="s">
         <v>235</v>
       </c>
-      <c r="F13" s="43" t="s">
+      <c r="F13" s="37" t="s">
         <v>315</v>
       </c>
-      <c r="H13" s="43" t="s">
+      <c r="H13" s="37" t="s">
         <v>252</v>
       </c>
-      <c r="I13" s="43">
+      <c r="I13" s="37">
         <v>6</v>
       </c>
-      <c r="J13" s="43" t="s">
+      <c r="J13" s="37" t="s">
         <v>253</v>
       </c>
-      <c r="K13" s="43" t="s">
+      <c r="K13" s="37" t="s">
         <v>254</v>
       </c>
-      <c r="L13" s="43" t="s">
+      <c r="L13" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="M13" s="43" t="s">
+      <c r="M13" s="37" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="37" t="s">
         <v>316</v>
       </c>
-      <c r="B14" s="43">
+      <c r="B14" s="37">
         <v>9</v>
       </c>
-      <c r="C14" s="43" t="s">
+      <c r="C14" s="37" t="s">
         <v>246</v>
       </c>
-      <c r="D14" s="43" t="s">
+      <c r="D14" s="37" t="s">
         <v>247</v>
       </c>
-      <c r="E14" s="43" t="s">
+      <c r="E14" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="43" t="s">
+      <c r="F14" s="37" t="s">
         <v>317</v>
       </c>
-      <c r="H14" s="43" t="s">
+      <c r="H14" s="37" t="s">
         <v>255</v>
       </c>
-      <c r="I14" s="43">
+      <c r="I14" s="37">
         <v>6</v>
       </c>
-      <c r="J14" s="43" t="s">
+      <c r="J14" s="37" t="s">
         <v>256</v>
       </c>
-      <c r="K14" s="43" t="s">
+      <c r="K14" s="37" t="s">
         <v>257</v>
       </c>
-      <c r="L14" s="43" t="s">
+      <c r="L14" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="M14" s="43" t="s">
+      <c r="M14" s="37" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="37" t="s">
         <v>318</v>
       </c>
-      <c r="B15" s="43">
+      <c r="B15" s="37">
         <v>9</v>
       </c>
-      <c r="C15" s="43" t="s">
+      <c r="C15" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="D15" s="43" t="s">
+      <c r="D15" s="37" t="s">
         <v>251</v>
       </c>
-      <c r="E15" s="43" t="s">
+      <c r="E15" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="F15" s="43" t="s">
+      <c r="F15" s="37" t="s">
         <v>317</v>
       </c>
-      <c r="H15" s="43" t="s">
+      <c r="H15" s="37" t="s">
         <v>258</v>
       </c>
-      <c r="I15" s="43">
+      <c r="I15" s="37">
         <v>4</v>
       </c>
-      <c r="J15" s="43" t="s">
+      <c r="J15" s="37" t="s">
         <v>259</v>
       </c>
-      <c r="K15" s="43" t="s">
+      <c r="K15" s="37" t="s">
         <v>260</v>
       </c>
-      <c r="L15" s="43" t="s">
+      <c r="L15" s="37" t="s">
         <v>181</v>
       </c>
-      <c r="M15" s="43" t="s">
+      <c r="M15" s="37" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="43" t="s">
+      <c r="A16" s="37" t="s">
         <v>319</v>
       </c>
-      <c r="B16" s="43">
+      <c r="B16" s="37">
         <v>6</v>
       </c>
-      <c r="C16" s="43" t="s">
+      <c r="C16" s="37" t="s">
         <v>253</v>
       </c>
-      <c r="D16" s="43" t="s">
+      <c r="D16" s="37" t="s">
         <v>254</v>
       </c>
-      <c r="E16" s="43" t="s">
+      <c r="E16" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="F16" s="43" t="s">
+      <c r="F16" s="37" t="s">
         <v>317</v>
       </c>
-      <c r="H16" s="43" t="s">
+      <c r="H16" s="37" t="s">
         <v>262</v>
       </c>
-      <c r="I16" s="43">
+      <c r="I16" s="37">
         <v>4</v>
       </c>
-      <c r="J16" s="43" t="s">
+      <c r="J16" s="37" t="s">
         <v>263</v>
       </c>
-      <c r="K16" s="43" t="s">
+      <c r="K16" s="37" t="s">
         <v>264</v>
       </c>
-      <c r="L16" s="43" t="s">
+      <c r="L16" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="M16" s="43" t="s">
+      <c r="M16" s="37" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="43" t="s">
+      <c r="A17" s="37" t="s">
         <v>320</v>
       </c>
-      <c r="B17" s="43">
+      <c r="B17" s="37">
         <v>6</v>
       </c>
-      <c r="C17" s="43" t="s">
+      <c r="C17" s="37" t="s">
         <v>256</v>
       </c>
-      <c r="D17" s="43" t="s">
+      <c r="D17" s="37" t="s">
         <v>257</v>
       </c>
-      <c r="E17" s="43" t="s">
+      <c r="E17" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="F17" s="43" t="s">
+      <c r="F17" s="37" t="s">
         <v>317</v>
       </c>
-      <c r="H17" s="43" t="s">
+      <c r="H17" s="37" t="s">
         <v>266</v>
       </c>
-      <c r="I17" s="43">
+      <c r="I17" s="37">
         <v>5</v>
       </c>
-      <c r="J17" s="43" t="s">
+      <c r="J17" s="37" t="s">
         <v>267</v>
       </c>
-      <c r="K17" s="43" t="s">
+      <c r="K17" s="37" t="s">
         <v>268</v>
       </c>
-      <c r="L17" s="43" t="s">
+      <c r="L17" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="M17" s="43" t="s">
+      <c r="M17" s="37" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="37" t="s">
         <v>321</v>
       </c>
-      <c r="B18" s="43">
+      <c r="B18" s="37">
         <v>30</v>
       </c>
-      <c r="C18" s="43" t="s">
+      <c r="C18" s="37" t="s">
         <v>322</v>
       </c>
-      <c r="D18" s="43" t="s">
+      <c r="D18" s="37" t="s">
         <v>323</v>
       </c>
-      <c r="E18" s="43" t="s">
+      <c r="E18" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="F18" s="43" t="s">
+      <c r="F18" s="37" t="s">
         <v>324</v>
       </c>
-      <c r="H18" s="43" t="s">
+      <c r="H18" s="37" t="s">
         <v>270</v>
       </c>
-      <c r="I18" s="43">
+      <c r="I18" s="37">
         <v>5</v>
       </c>
-      <c r="J18" s="43" t="s">
+      <c r="J18" s="37" t="s">
         <v>271</v>
       </c>
-      <c r="K18" s="43" t="s">
+      <c r="K18" s="37" t="s">
         <v>272</v>
       </c>
-      <c r="L18" s="43" t="s">
+      <c r="L18" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="M18" s="43" t="s">
+      <c r="M18" s="37" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="37" t="s">
         <v>325</v>
       </c>
-      <c r="B19" s="43">
+      <c r="B19" s="37">
         <v>6</v>
       </c>
-      <c r="C19" s="43" t="s">
+      <c r="C19" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="D19" s="46"/>
-      <c r="E19" s="43" t="s">
+      <c r="D19" s="40"/>
+      <c r="E19" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="F19" s="43" t="s">
+      <c r="F19" s="37" t="s">
         <v>326</v>
       </c>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>274</v>
       </c>
-      <c r="I19" s="43">
+      <c r="I19" s="37">
         <v>6</v>
       </c>
-      <c r="J19" s="43" t="s">
+      <c r="J19" s="37" t="s">
         <v>275</v>
       </c>
-      <c r="K19" s="43" t="s">
+      <c r="K19" s="37" t="s">
         <v>276</v>
       </c>
-      <c r="L19" s="43" t="s">
+      <c r="L19" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="M19" s="43" t="s">
+      <c r="M19" s="37" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H20" s="43" t="s">
+      <c r="H20" s="37" t="s">
         <v>278</v>
       </c>
-      <c r="I20" s="43">
+      <c r="I20" s="37">
         <v>8</v>
       </c>
-      <c r="J20" s="43" t="s">
+      <c r="J20" s="37" t="s">
         <v>279</v>
       </c>
-      <c r="K20" s="43" t="s">
+      <c r="K20" s="37" t="s">
         <v>280</v>
       </c>
-      <c r="L20" s="43" t="s">
+      <c r="L20" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="M20" s="43" t="s">
+      <c r="M20" s="37" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H21" s="43" t="s">
+      <c r="H21" s="37" t="s">
         <v>282</v>
       </c>
-      <c r="I21" s="43">
+      <c r="I21" s="37">
         <v>120</v>
       </c>
-      <c r="J21" s="43" t="s">
+      <c r="J21" s="37" t="s">
         <v>283</v>
       </c>
-      <c r="K21" s="43" t="s">
+      <c r="K21" s="37" t="s">
         <v>284</v>
       </c>
-      <c r="L21" s="43" t="s">
+      <c r="L21" s="37" t="s">
         <v>235</v>
       </c>
-      <c r="M21" s="43" t="s">
+      <c r="M21" s="37" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H22" s="43" t="s">
+      <c r="H22" s="37" t="s">
         <v>286</v>
       </c>
-      <c r="I22" s="43">
+      <c r="I22" s="37">
         <v>1</v>
       </c>
-      <c r="J22" s="43" t="s">
+      <c r="J22" s="37" t="s">
         <v>287</v>
       </c>
-      <c r="K22" s="43" t="s">
+      <c r="K22" s="37" t="s">
         <v>288</v>
       </c>
-      <c r="L22" s="43" t="s">
+      <c r="L22" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="M22" s="43" t="s">
+      <c r="M22" s="37" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="H23" s="43" t="s">
+      <c r="H23" s="37" t="s">
         <v>290</v>
       </c>
-      <c r="I23" s="43">
+      <c r="I23" s="37">
         <v>1</v>
       </c>
-      <c r="J23" s="43" t="s">
+      <c r="J23" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="K23" s="46"/>
-      <c r="L23" s="43" t="s">
+      <c r="K23" s="40"/>
+      <c r="L23" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="M23" s="43" t="s">
+      <c r="M23" s="37" t="s">
         <v>72</v>
       </c>
     </row>
@@ -4717,32 +4723,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="62" t="s">
         <v>219</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
     </row>
     <row r="2" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="20" t="s">
         <v>220</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="20" t="s">
         <v>221</v>
       </c>
     </row>
@@ -4767,7 +4773,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="21" t="s">
         <v>60</v>
       </c>
       <c r="B4" s="18">
@@ -4787,7 +4793,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="21" t="s">
         <v>64</v>
       </c>
       <c r="B5" s="18">
@@ -4822,7 +4828,7 @@
       <c r="E6" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="24" t="s">
+      <c r="F6" s="22" t="s">
         <v>227</v>
       </c>
     </row>
@@ -5156,7 +5162,7 @@
       <c r="C23" s="18" t="s">
         <v>214</v>
       </c>
-      <c r="D23" s="32"/>
+      <c r="D23" s="27"/>
       <c r="E23" s="18" t="s">
         <v>71</v>
       </c>

</xml_diff>

<commit_message>
message ais 18 cleaned up and verified (+1 type)
</commit_message>
<xml_diff>
--- a/test_bl/resources/tests/TrassaTests_v01.xlsx
+++ b/test_bl/resources/tests/TrassaTests_v01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13380" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13380" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="trassa_Tests" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="400">
   <si>
     <t>1.1.1</t>
   </si>
@@ -1302,12 +1302,78 @@
 сообщения AIVDM (5, 24) (см. Таблицу $PAIDD)
 2) В логах КД выявить сообщение об ошибке</t>
   </si>
+  <si>
+    <t>- MessageID(uint): AIS message number.  Must be 18 (field automatically set to "18")</t>
+  </si>
+  <si>
+    <t>- RepeatIndicator(uint): Indicated how many times a message has been repeated</t>
+  </si>
+  <si>
+    <t>- UserID(uint): Unique ship identification number (MMSI)</t>
+  </si>
+  <si>
+    <t>- Reserved1(uint): Reseverd for definition by a compentent regional or local authority.  Should be set to zero. (field automatically set to "0")</t>
+  </si>
+  <si>
+    <t>- SOG(udecimal): Speed over ground</t>
+  </si>
+  <si>
+    <t>- PositionAccuracy(uint): Accuracy of positioning fixes</t>
+  </si>
+  <si>
+    <t>- longitude(decimal): Location of the vessel  East West location</t>
+  </si>
+  <si>
+    <t>- latitude(decimal): Location of the vessel  North South location</t>
+  </si>
+  <si>
+    <t>- COG(udecimal): Course over ground</t>
+  </si>
+  <si>
+    <t>- TrueHeading(uint): True heading (relative to true North)</t>
+  </si>
+  <si>
+    <t>- TimeStamp(uint): UTC second when the report was generated</t>
+  </si>
+  <si>
+    <t>- Spare(uint): Not used.  Should be set to zero. (field automatically set to "0")</t>
+  </si>
+  <si>
+    <t>- cs_unit(bool): Does this unit do Carrier Sense?</t>
+  </si>
+  <si>
+    <t>- display_flag(bool): Does this class B unit have an integrated display?</t>
+  </si>
+  <si>
+    <t>- dsc_flag(bool): Does it have dedicated or time-shared DSC radio function?</t>
+  </si>
+  <si>
+    <t>- band_flag(bool): How flexible is the freq handling of the unit?</t>
+  </si>
+  <si>
+    <t>- msg22_flag(bool): Can the unit handle msg 22?</t>
+  </si>
+  <si>
+    <t>- mode_flag(bool): Assigned mode wrt to VDL slots</t>
+  </si>
+  <si>
+    <t>- RAIM(bool): Receiver autonomous integrity monitoring flag</t>
+  </si>
+  <si>
+    <t>- CommStateSelector(uint): SOTDMA or ITDMA</t>
+  </si>
+  <si>
+    <t>- CommState(uint): Not decoded by this software yet</t>
+  </si>
+  <si>
+    <t>AIS LIB FILELDS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1396,6 +1462,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Fira Code"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1500,7 +1571,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1671,6 +1742,18 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1679,17 +1762,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2098,7 +2172,7 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="1"/>
     <col min="2" max="2" width="47" style="1" customWidth="1"/>
@@ -2111,7 +2185,7 @@
     <col min="9" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8">
       <c r="A2" s="54" t="s">
         <v>7</v>
       </c>
@@ -2137,7 +2211,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="159.5">
       <c r="A3" s="31">
         <v>1</v>
       </c>
@@ -2159,7 +2233,7 @@
       <c r="G3" s="33"/>
       <c r="H3" s="34"/>
     </row>
-    <row r="4" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="87">
       <c r="A4" s="31">
         <v>2</v>
       </c>
@@ -2181,7 +2255,7 @@
       <c r="G4" s="33"/>
       <c r="H4" s="34"/>
     </row>
-    <row r="5" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="58">
       <c r="A5" s="31">
         <v>3</v>
       </c>
@@ -2201,7 +2275,7 @@
       <c r="G5" s="33"/>
       <c r="H5" s="34"/>
     </row>
-    <row r="6" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="58">
       <c r="A6" s="31">
         <v>4</v>
       </c>
@@ -2221,7 +2295,7 @@
       <c r="G6" s="33"/>
       <c r="H6" s="34"/>
     </row>
-    <row r="7" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="87">
       <c r="A7" s="31">
         <v>5</v>
       </c>
@@ -2243,7 +2317,7 @@
       <c r="G7" s="33"/>
       <c r="H7" s="34"/>
     </row>
-    <row r="8" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="72.5">
       <c r="A8" s="31">
         <v>6</v>
       </c>
@@ -2263,7 +2337,7 @@
       <c r="G8" s="33"/>
       <c r="H8" s="34"/>
     </row>
-    <row r="9" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" ht="58">
       <c r="A9" s="54">
         <v>7</v>
       </c>
@@ -2283,7 +2357,7 @@
       <c r="G9" s="57"/>
       <c r="H9" s="58"/>
     </row>
-    <row r="10" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="58">
       <c r="A10" s="54">
         <v>8</v>
       </c>
@@ -2303,7 +2377,7 @@
       <c r="G10" s="57"/>
       <c r="H10" s="58"/>
     </row>
-    <row r="11" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="72.5">
       <c r="A11" s="54">
         <v>9</v>
       </c>
@@ -2323,7 +2397,7 @@
       <c r="G11" s="57"/>
       <c r="H11" s="58"/>
     </row>
-    <row r="12" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="58">
       <c r="A12" s="54">
         <v>10</v>
       </c>
@@ -2343,7 +2417,7 @@
       <c r="G12" s="58"/>
       <c r="H12" s="58"/>
     </row>
-    <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="43.5">
       <c r="A13" s="54">
         <v>11</v>
       </c>
@@ -2361,7 +2435,7 @@
       <c r="G13" s="58"/>
       <c r="H13" s="58"/>
     </row>
-    <row r="14" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="43.5">
       <c r="A14" s="54">
         <v>12</v>
       </c>
@@ -2379,7 +2453,7 @@
       <c r="G14" s="58"/>
       <c r="H14" s="58"/>
     </row>
-    <row r="15" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" ht="43.5">
       <c r="A15" s="54">
         <v>13</v>
       </c>
@@ -2411,7 +2485,7 @@
       <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="31.453125" customWidth="1"/>
     <col min="2" max="2" width="37.90625" customWidth="1"/>
@@ -2421,7 +2495,7 @@
     <col min="6" max="6" width="25.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -2429,7 +2503,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6">
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
@@ -2437,7 +2511,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6">
       <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
@@ -2445,7 +2519,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6">
       <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
@@ -2465,7 +2539,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -2473,7 +2547,7 @@
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6">
       <c r="A6" s="9" t="s">
         <v>7</v>
       </c>
@@ -2481,7 +2555,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6">
       <c r="A7" s="9" t="s">
         <v>8</v>
       </c>
@@ -2489,7 +2563,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6">
       <c r="A8" s="9" t="s">
         <v>9</v>
       </c>
@@ -2497,7 +2571,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6">
       <c r="A9" s="9" t="s">
         <v>10</v>
       </c>
@@ -2505,7 +2579,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6">
       <c r="A10" s="9" t="s">
         <v>11</v>
       </c>
@@ -2513,7 +2587,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6">
       <c r="A11" s="9" t="s">
         <v>12</v>
       </c>
@@ -2521,25 +2595,25 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6">
       <c r="A13" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="10"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6">
       <c r="A14" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="10"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6">
       <c r="A15" s="10" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="10"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6">
       <c r="A16" s="11" t="s">
         <v>22</v>
       </c>
@@ -2547,7 +2621,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7">
       <c r="A17" s="12" t="s">
         <v>24</v>
       </c>
@@ -2555,7 +2629,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7">
       <c r="A18" s="13" t="s">
         <v>26</v>
       </c>
@@ -2563,12 +2637,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7">
       <c r="A21" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7">
       <c r="A22" s="7" t="s">
         <v>7</v>
       </c>
@@ -2589,7 +2663,7 @@
       </c>
       <c r="G22" s="14"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7">
       <c r="A23" s="8">
         <v>1</v>
       </c>
@@ -2604,7 +2678,7 @@
       <c r="F23" s="8"/>
       <c r="G23" s="14"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7">
       <c r="A24" s="14">
         <v>2</v>
       </c>
@@ -2619,7 +2693,7 @@
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7">
       <c r="A25" s="14">
         <v>3</v>
       </c>
@@ -2638,7 +2712,7 @@
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7">
       <c r="A26" s="14"/>
       <c r="B26" s="16" t="s">
         <v>35</v>
@@ -2659,7 +2733,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7">
       <c r="A27" s="14"/>
       <c r="B27" s="16" t="s">
         <v>39</v>
@@ -2676,16 +2750,16 @@
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7">
       <c r="B28" s="16"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7">
       <c r="B29" s="16"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7">
       <c r="B30" s="16"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7">
       <c r="B31" s="16"/>
     </row>
   </sheetData>
@@ -2705,7 +2779,7 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="13.90625" style="2" customWidth="1"/>
     <col min="2" max="2" width="32.36328125" style="1" customWidth="1"/>
@@ -2714,7 +2788,7 @@
     <col min="5" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="43" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="43" customFormat="1" ht="15.5">
       <c r="A1" s="46" t="s">
         <v>138</v>
       </c>
@@ -2725,7 +2799,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" s="4" customFormat="1" ht="43.5">
       <c r="A2" s="44" t="s">
         <v>139</v>
       </c>
@@ -2736,7 +2810,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4">
       <c r="A3" s="44" t="s">
         <v>140</v>
       </c>
@@ -2747,7 +2821,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4">
       <c r="A4" s="45" t="s">
         <v>141</v>
       </c>
@@ -2758,7 +2832,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4">
       <c r="A5" s="44" t="s">
         <v>142</v>
       </c>
@@ -2769,7 +2843,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4">
       <c r="A6" s="44" t="s">
         <v>143</v>
       </c>
@@ -2780,7 +2854,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="29">
       <c r="A7" s="44" t="s">
         <v>144</v>
       </c>
@@ -2794,7 +2868,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4">
       <c r="A8" s="44" t="s">
         <v>145</v>
       </c>
@@ -2805,7 +2879,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="29">
       <c r="A9" s="44" t="s">
         <v>146</v>
       </c>
@@ -2816,7 +2890,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4">
       <c r="A10" s="44" t="s">
         <v>343</v>
       </c>
@@ -2827,7 +2901,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="29">
       <c r="A11" s="44" t="s">
         <v>344</v>
       </c>
@@ -2835,7 +2909,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
         <v>163</v>
       </c>
@@ -2850,11 +2924,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="10.26953125" style="28" customWidth="1"/>
     <col min="2" max="2" width="8.7265625" style="3"/>
@@ -2867,30 +2941,30 @@
     <col min="9" max="9" width="50.08984375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="55" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="65" t="s">
+    <row r="1" spans="1:9" ht="55" customHeight="1">
+      <c r="A1" s="61" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-    </row>
-    <row r="2" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="59" t="s">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+    </row>
+    <row r="2" spans="1:9" ht="16" thickBot="1">
+      <c r="A2" s="63" t="s">
         <v>170</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
       <c r="H2" s="24" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" ht="18" thickBot="1">
       <c r="A3" s="25" t="s">
         <v>49</v>
       </c>
@@ -2906,7 +2980,7 @@
       <c r="E3" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="63" t="s">
+      <c r="F3" s="59" t="s">
         <v>54</v>
       </c>
       <c r="H3" s="18">
@@ -2916,7 +2990,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" ht="18" thickBot="1">
       <c r="A4" s="26" t="s">
         <v>55</v>
       </c>
@@ -2932,7 +3006,7 @@
       <c r="E4" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="64" t="s">
+      <c r="F4" s="60" t="s">
         <v>173</v>
       </c>
       <c r="H4" s="18">
@@ -2942,7 +3016,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" ht="18" thickBot="1">
       <c r="A5" s="26">
         <v>43287</v>
       </c>
@@ -2958,7 +3032,7 @@
       <c r="E5" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="64" t="s">
+      <c r="F5" s="60" t="s">
         <v>175</v>
       </c>
       <c r="H5" s="18">
@@ -2968,7 +3042,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" ht="18" thickBot="1">
       <c r="A6" s="26">
         <v>13728</v>
       </c>
@@ -2984,7 +3058,7 @@
       <c r="E6" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="64" t="s">
+      <c r="F6" s="60" t="s">
         <v>67</v>
       </c>
       <c r="H6" s="18">
@@ -2994,7 +3068,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" ht="18" thickBot="1">
       <c r="A7" s="26" t="s">
         <v>178</v>
       </c>
@@ -3010,7 +3084,7 @@
       <c r="E7" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="F7" s="64" t="s">
+      <c r="F7" s="60" t="s">
         <v>182</v>
       </c>
       <c r="H7" s="18">
@@ -3020,7 +3094,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9" ht="35.5" thickBot="1">
       <c r="A8" s="26" t="s">
         <v>184</v>
       </c>
@@ -3036,7 +3110,7 @@
       <c r="E8" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="F8" s="64" t="s">
+      <c r="F8" s="60" t="s">
         <v>81</v>
       </c>
       <c r="H8" s="18">
@@ -3046,7 +3120,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" ht="35.5" thickBot="1">
       <c r="A9" s="26" t="s">
         <v>189</v>
       </c>
@@ -3062,7 +3136,7 @@
       <c r="E9" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="F9" s="64" t="s">
+      <c r="F9" s="60" t="s">
         <v>81</v>
       </c>
       <c r="H9" s="18">
@@ -3072,7 +3146,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9" ht="18" thickBot="1">
       <c r="A10" s="26" t="s">
         <v>192</v>
       </c>
@@ -3088,7 +3162,7 @@
       <c r="E10" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="F10" s="64" t="s">
+      <c r="F10" s="60" t="s">
         <v>81</v>
       </c>
       <c r="H10" s="18">
@@ -3098,7 +3172,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" ht="18" thickBot="1">
       <c r="A11" s="26" t="s">
         <v>194</v>
       </c>
@@ -3114,7 +3188,7 @@
       <c r="E11" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="F11" s="64" t="s">
+      <c r="F11" s="60" t="s">
         <v>195</v>
       </c>
       <c r="H11" s="18">
@@ -3124,7 +3198,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" ht="35.5" thickBot="1">
       <c r="A12" s="26" t="s">
         <v>197</v>
       </c>
@@ -3140,7 +3214,7 @@
       <c r="E12" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="F12" s="64" t="s">
+      <c r="F12" s="60" t="s">
         <v>195</v>
       </c>
       <c r="H12" s="18">
@@ -3150,7 +3224,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" ht="35.5" thickBot="1">
       <c r="A13" s="26" t="s">
         <v>199</v>
       </c>
@@ -3166,7 +3240,7 @@
       <c r="E13" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="F13" s="64" t="s">
+      <c r="F13" s="60" t="s">
         <v>201</v>
       </c>
       <c r="H13" s="18">
@@ -3176,7 +3250,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9" ht="35.5" thickBot="1">
       <c r="A14" s="26" t="s">
         <v>203</v>
       </c>
@@ -3192,7 +3266,7 @@
       <c r="E14" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="64" t="s">
+      <c r="F14" s="60" t="s">
         <v>205</v>
       </c>
       <c r="H14" s="18">
@@ -3202,7 +3276,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" ht="18" thickBot="1">
       <c r="A15" s="26" t="s">
         <v>207</v>
       </c>
@@ -3218,7 +3292,7 @@
       <c r="E15" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="F15" s="64" t="s">
+      <c r="F15" s="60" t="s">
         <v>208</v>
       </c>
       <c r="H15" s="18">
@@ -3228,7 +3302,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" ht="35.5" thickBot="1">
       <c r="A16" s="26" t="s">
         <v>209</v>
       </c>
@@ -3244,7 +3318,7 @@
       <c r="E16" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="F16" s="64" t="s">
+      <c r="F16" s="60" t="s">
         <v>212</v>
       </c>
       <c r="H16" s="18">
@@ -3254,7 +3328,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" ht="18" thickBot="1">
       <c r="A17" s="26" t="s">
         <v>213</v>
       </c>
@@ -3268,7 +3342,7 @@
       <c r="E17" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="F17" s="64" t="s">
+      <c r="F17" s="60" t="s">
         <v>72</v>
       </c>
       <c r="H17" s="18">
@@ -3278,7 +3352,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" ht="18" thickBot="1">
       <c r="A18" s="26" t="s">
         <v>216</v>
       </c>
@@ -3294,7 +3368,7 @@
       <c r="E18" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="F18" s="64" t="s">
+      <c r="F18" s="60" t="s">
         <v>81</v>
       </c>
       <c r="H18" s="18">
@@ -3304,7 +3378,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" ht="18" thickBot="1">
       <c r="A19" s="26" t="s">
         <v>218</v>
       </c>
@@ -3320,7 +3394,7 @@
       <c r="E19" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="F19" s="64" t="s">
+      <c r="F19" s="60" t="s">
         <v>81</v>
       </c>
     </row>
@@ -3336,40 +3410,42 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="26.36328125" style="23" customWidth="1"/>
     <col min="2" max="2" width="8.7265625" style="23"/>
     <col min="3" max="3" width="28.1796875" style="23" customWidth="1"/>
     <col min="4" max="5" width="8.7265625" style="23"/>
     <col min="6" max="6" width="54.1796875" style="23" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="19"/>
+    <col min="7" max="7" width="8.7265625" style="19"/>
+    <col min="8" max="8" width="158.54296875" style="19" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="60" t="s">
+    <row r="1" spans="1:13" ht="15" thickBot="1">
+      <c r="A1" s="64" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-    </row>
-    <row r="2" spans="1:13" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+    </row>
+    <row r="2" spans="1:13" ht="35.5" thickBot="1">
       <c r="A2" s="20" t="s">
         <v>49</v>
       </c>
@@ -3388,8 +3464,11 @@
       <c r="F2" s="20" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H2" s="19" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="18" thickBot="1">
       <c r="A3" s="18" t="s">
         <v>55</v>
       </c>
@@ -3408,8 +3487,11 @@
       <c r="F3" s="18" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H3" s="67" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="18" thickBot="1">
       <c r="A4" s="21" t="s">
         <v>60</v>
       </c>
@@ -3428,8 +3510,11 @@
       <c r="F4" s="18" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H4" s="67" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="18" thickBot="1">
       <c r="A5" s="21" t="s">
         <v>64</v>
       </c>
@@ -3448,8 +3533,11 @@
       <c r="F5" s="18" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H5" s="67" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="35.5" thickBot="1">
       <c r="A6" s="18" t="s">
         <v>68</v>
       </c>
@@ -3468,8 +3556,11 @@
       <c r="F6" s="18" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H6" s="67" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="18" thickBot="1">
       <c r="A7" s="18" t="s">
         <v>73</v>
       </c>
@@ -3488,8 +3579,11 @@
       <c r="F7" s="18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H7" s="67" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="35.5" thickBot="1">
       <c r="A8" s="18" t="s">
         <v>78</v>
       </c>
@@ -3508,8 +3602,11 @@
       <c r="F8" s="18" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H8" s="67" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="18" thickBot="1">
       <c r="A9" s="18" t="s">
         <v>82</v>
       </c>
@@ -3528,8 +3625,11 @@
       <c r="F9" s="18" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H9" s="67" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="18" thickBot="1">
       <c r="A10" s="18" t="s">
         <v>87</v>
       </c>
@@ -3548,8 +3648,11 @@
       <c r="F10" s="18" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H10" s="67" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="18" thickBot="1">
       <c r="A11" s="18" t="s">
         <v>90</v>
       </c>
@@ -3568,8 +3671,11 @@
       <c r="F11" s="18" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H11" s="67" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="35.5" thickBot="1">
       <c r="A12" s="18" t="s">
         <v>94</v>
       </c>
@@ -3588,8 +3694,11 @@
       <c r="F12" s="18" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H12" s="67" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="35.5" thickBot="1">
       <c r="A13" s="18" t="s">
         <v>98</v>
       </c>
@@ -3608,8 +3717,11 @@
       <c r="F13" s="18" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H13" s="67" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="35.5" thickBot="1">
       <c r="A14" s="18" t="s">
         <v>102</v>
       </c>
@@ -3628,8 +3740,11 @@
       <c r="F14" s="18" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H14" s="67" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="35.5" thickBot="1">
       <c r="A15" s="18" t="s">
         <v>106</v>
       </c>
@@ -3648,8 +3763,11 @@
       <c r="F15" s="18" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H15" s="67" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="35.5" thickBot="1">
       <c r="A16" s="18" t="s">
         <v>110</v>
       </c>
@@ -3668,8 +3786,11 @@
       <c r="F16" s="18" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H16" s="67" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="35.5" thickBot="1">
       <c r="A17" s="18" t="s">
         <v>114</v>
       </c>
@@ -3688,8 +3809,11 @@
       <c r="F17" s="18" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="53" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H17" s="67" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="53" thickBot="1">
       <c r="A18" s="18" t="s">
         <v>118</v>
       </c>
@@ -3708,8 +3832,11 @@
       <c r="F18" s="18" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H18" s="67" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="35.5" thickBot="1">
       <c r="A19" s="18" t="s">
         <v>122</v>
       </c>
@@ -3728,8 +3855,11 @@
       <c r="F19" s="18" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H19" s="67" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="35.5" thickBot="1">
       <c r="A20" s="18" t="s">
         <v>126</v>
       </c>
@@ -3748,8 +3878,11 @@
       <c r="F20" s="18" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H20" s="67" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="18" thickBot="1">
       <c r="A21" s="18" t="s">
         <v>130</v>
       </c>
@@ -3768,8 +3901,11 @@
       <c r="F21" s="18" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H21" s="67" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="18" thickBot="1">
       <c r="A22" s="18" t="s">
         <v>134</v>
       </c>
@@ -3787,6 +3923,14 @@
       </c>
       <c r="F22" s="22" t="s">
         <v>137</v>
+      </c>
+      <c r="H22" s="67" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="H23" s="67" t="s">
+        <v>398</v>
       </c>
     </row>
   </sheetData>
@@ -3797,6 +3941,7 @@
     <hyperlink ref="F22" r:id="rId1" location="IALA" display="http://catb.org/gpsd/AIVDM.html - IALA"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3808,7 +3953,7 @@
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="48"/>
     <col min="2" max="2" width="17.90625" style="4" customWidth="1"/>
@@ -3818,7 +3963,7 @@
     <col min="6" max="16384" width="8.7265625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" s="51" t="s">
         <v>157</v>
       </c>
@@ -3830,7 +3975,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="58">
       <c r="A2" s="49" t="s">
         <v>158</v>
       </c>
@@ -3841,7 +3986,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="58">
       <c r="A3" s="49" t="s">
         <v>159</v>
       </c>
@@ -3855,7 +4000,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="72.5">
       <c r="A4" s="49" t="s">
         <v>160</v>
       </c>
@@ -3866,7 +4011,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="72.5">
       <c r="A5" s="49" t="s">
         <v>161</v>
       </c>
@@ -3877,7 +4022,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="43.5">
       <c r="A6" s="49" t="s">
         <v>162</v>
       </c>
@@ -3886,7 +4031,7 @@
       </c>
       <c r="C6" s="30"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4">
       <c r="A7" s="49" t="s">
         <v>163</v>
       </c>
@@ -3907,7 +4052,7 @@
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="19.7265625" style="23" customWidth="1"/>
     <col min="2" max="2" width="8.7265625" style="23"/>
@@ -3925,7 +4070,7 @@
     <col min="14" max="16384" width="8.7265625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="15" customHeight="1" thickBot="1">
       <c r="A1" s="23" t="s">
         <v>291</v>
       </c>
@@ -3938,7 +4083,7 @@
       <c r="L1" s="41"/>
       <c r="M1" s="41"/>
     </row>
-    <row r="2" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" ht="18" thickBot="1">
       <c r="A2" s="36" t="s">
         <v>49</v>
       </c>
@@ -3976,7 +4121,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" ht="18" thickBot="1">
       <c r="A3" s="37" t="s">
         <v>55</v>
       </c>
@@ -4014,7 +4159,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" ht="18" thickBot="1">
       <c r="A4" s="38" t="s">
         <v>60</v>
       </c>
@@ -4052,7 +4197,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" ht="18" thickBot="1">
       <c r="A5" s="38" t="s">
         <v>64</v>
       </c>
@@ -4090,7 +4235,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" ht="18" thickBot="1">
       <c r="A6" s="37" t="s">
         <v>224</v>
       </c>
@@ -4128,7 +4273,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:13" ht="18" thickBot="1">
       <c r="A7" s="37" t="s">
         <v>297</v>
       </c>
@@ -4166,7 +4311,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:13" ht="18" thickBot="1">
       <c r="A8" s="37" t="s">
         <v>299</v>
       </c>
@@ -4202,7 +4347,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:13" ht="18" thickBot="1">
       <c r="A9" s="37" t="s">
         <v>301</v>
       </c>
@@ -4240,7 +4385,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" ht="18" thickBot="1">
       <c r="A10" s="37" t="s">
         <v>303</v>
       </c>
@@ -4278,7 +4423,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:13" ht="18" thickBot="1">
       <c r="A11" s="37" t="s">
         <v>307</v>
       </c>
@@ -4316,7 +4461,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:13" ht="18" thickBot="1">
       <c r="A12" s="37" t="s">
         <v>311</v>
       </c>
@@ -4354,7 +4499,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:13" ht="18" thickBot="1">
       <c r="A13" s="37" t="s">
         <v>314</v>
       </c>
@@ -4392,7 +4537,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:13" ht="18" thickBot="1">
       <c r="A14" s="37" t="s">
         <v>316</v>
       </c>
@@ -4430,7 +4575,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:13" ht="18" thickBot="1">
       <c r="A15" s="37" t="s">
         <v>318</v>
       </c>
@@ -4468,7 +4613,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:13" ht="18" thickBot="1">
       <c r="A16" s="37" t="s">
         <v>319</v>
       </c>
@@ -4506,7 +4651,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:13" ht="18" thickBot="1">
       <c r="A17" s="37" t="s">
         <v>320</v>
       </c>
@@ -4544,7 +4689,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:13" ht="18" thickBot="1">
       <c r="A18" s="37" t="s">
         <v>321</v>
       </c>
@@ -4582,7 +4727,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:13" ht="18" thickBot="1">
       <c r="A19" s="37" t="s">
         <v>325</v>
       </c>
@@ -4618,7 +4763,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:13" ht="18" thickBot="1">
       <c r="H20" s="37" t="s">
         <v>278</v>
       </c>
@@ -4638,7 +4783,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:13" ht="18" thickBot="1">
       <c r="H21" s="37" t="s">
         <v>282</v>
       </c>
@@ -4658,7 +4803,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:13" ht="18" thickBot="1">
       <c r="H22" s="37" t="s">
         <v>286</v>
       </c>
@@ -4678,7 +4823,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:13" ht="18" thickBot="1">
       <c r="H23" s="37" t="s">
         <v>290</v>
       </c>
@@ -4712,7 +4857,7 @@
       <selection sqref="A1:F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="9.90625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.7265625" style="3"/>
@@ -4722,17 +4867,17 @@
     <col min="6" max="6" width="52.26953125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="62" t="s">
+    <row r="1" spans="1:6" ht="15" thickBot="1">
+      <c r="A1" s="66" t="s">
         <v>219</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-    </row>
-    <row r="2" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+    </row>
+    <row r="2" spans="1:6" ht="35.5" thickBot="1">
       <c r="A2" s="20" t="s">
         <v>49</v>
       </c>
@@ -4752,7 +4897,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" ht="18" thickBot="1">
       <c r="A3" s="18" t="s">
         <v>55</v>
       </c>
@@ -4772,7 +4917,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" ht="18" thickBot="1">
       <c r="A4" s="21" t="s">
         <v>60</v>
       </c>
@@ -4792,7 +4937,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" ht="18" thickBot="1">
       <c r="A5" s="21" t="s">
         <v>64</v>
       </c>
@@ -4812,7 +4957,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" ht="18" thickBot="1">
       <c r="A6" s="18" t="s">
         <v>224</v>
       </c>
@@ -4832,7 +4977,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" ht="18" thickBot="1">
       <c r="A7" s="18" t="s">
         <v>228</v>
       </c>
@@ -4852,7 +4997,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" ht="18" thickBot="1">
       <c r="A8" s="18" t="s">
         <v>232</v>
       </c>
@@ -4872,7 +5017,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" ht="18" thickBot="1">
       <c r="A9" s="18" t="s">
         <v>237</v>
       </c>
@@ -4892,7 +5037,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" ht="35.5" thickBot="1">
       <c r="A10" s="18" t="s">
         <v>241</v>
       </c>
@@ -4912,7 +5057,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" ht="35.5" thickBot="1">
       <c r="A11" s="18" t="s">
         <v>245</v>
       </c>
@@ -4932,7 +5077,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" ht="35.5" thickBot="1">
       <c r="A12" s="18" t="s">
         <v>249</v>
       </c>
@@ -4952,7 +5097,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" ht="35.5" thickBot="1">
       <c r="A13" s="18" t="s">
         <v>252</v>
       </c>
@@ -4972,7 +5117,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" ht="35.5" thickBot="1">
       <c r="A14" s="18" t="s">
         <v>255</v>
       </c>
@@ -4992,7 +5137,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" ht="35.5" thickBot="1">
       <c r="A15" s="18" t="s">
         <v>258</v>
       </c>
@@ -5012,7 +5157,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" ht="35.5" thickBot="1">
       <c r="A16" s="18" t="s">
         <v>262</v>
       </c>
@@ -5032,7 +5177,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" ht="35.5" thickBot="1">
       <c r="A17" s="18" t="s">
         <v>266</v>
       </c>
@@ -5052,7 +5197,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:6" ht="35.5" thickBot="1">
       <c r="A18" s="18" t="s">
         <v>270</v>
       </c>
@@ -5072,7 +5217,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:6" ht="35.5" thickBot="1">
       <c r="A19" s="18" t="s">
         <v>274</v>
       </c>
@@ -5092,7 +5237,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:6" ht="35.5" thickBot="1">
       <c r="A20" s="18" t="s">
         <v>278</v>
       </c>
@@ -5112,7 +5257,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:6" ht="35.5" thickBot="1">
       <c r="A21" s="18" t="s">
         <v>282</v>
       </c>
@@ -5132,7 +5277,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:6" ht="35.5" thickBot="1">
       <c r="A22" s="18" t="s">
         <v>286</v>
       </c>
@@ -5152,7 +5297,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:6" ht="35.5" thickBot="1">
       <c r="A23" s="18" t="s">
         <v>290</v>
       </c>

</xml_diff>

<commit_message>
added structures to nmeautils (modified pynmea2 to generate: aitxt aialr pcmst
paisd (to be used for parsing)
paidd (to be used for parsing)
</commit_message>
<xml_diff>
--- a/test_bl/resources/tests/TrassaTests_v01.xlsx
+++ b/test_bl/resources/tests/TrassaTests_v01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13380" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13380" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="trassa_Tests" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="379">
   <si>
     <t>1.1.1</t>
   </si>
@@ -448,60 +448,6 @@
   </si>
   <si>
     <t>$PAIDD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1)xxxxxxx </t>
-  </si>
-  <si>
-    <t>(2)llll.ll</t>
-  </si>
-  <si>
-    <t>(3)a</t>
-  </si>
-  <si>
-    <t>(4)yyyyy.y</t>
-  </si>
-  <si>
-    <t>(5)a</t>
-  </si>
-  <si>
-    <t>(6)x.x</t>
-  </si>
-  <si>
-    <t>(7)x.x</t>
-  </si>
-  <si>
-    <t>(8)x.x</t>
-  </si>
-  <si>
-    <t>1-  идентификатор сопровождаемого АИС суднав МПС (MMSI)</t>
-  </si>
-  <si>
-    <t>2-  широта</t>
-  </si>
-  <si>
-    <t>3-  признак полушария "N","S"</t>
-  </si>
-  <si>
-    <t>4-  долгота</t>
-  </si>
-  <si>
-    <t>5-  признак полушария"E","W"</t>
-  </si>
-  <si>
-    <t>6-  скорость судна относительно грунта в узлах</t>
-  </si>
-  <si>
-    <t>7-  путевой угол судна в градусах</t>
-  </si>
-  <si>
-    <t>8-  курс судна в градусах (истинный)</t>
-  </si>
-  <si>
-    <t>9-  время получения данных (UTC)</t>
-  </si>
-  <si>
-    <t>10- контрольная сумма предложения</t>
   </si>
   <si>
     <t>$PAISD</t>
@@ -1090,28 +1036,10 @@
     <t>(9) hhmmss.ss</t>
   </si>
   <si>
-    <t>(10)*hh</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Field: MMSI</t>
-  </si>
-  <si>
     <t>AIVDM type 1 or 18</t>
   </si>
   <si>
-    <t>Field: Longitude</t>
-  </si>
-  <si>
     <t>Calculated in plugin</t>
-  </si>
-  <si>
-    <t>Field: Speed Over Ground</t>
-  </si>
-  <si>
-    <t>Field: Latitude</t>
-  </si>
-  <si>
-    <t>Field:True Heading (HDG)</t>
   </si>
   <si>
     <t>Проверка передачи информации о статусе судна из изделия "Трасса"
@@ -1142,9 +1070,6 @@
   </si>
   <si>
     <t>Field: Call Sign</t>
-  </si>
-  <si>
-    <t>Field: Vessel Nam</t>
   </si>
   <si>
     <t>1) Поля из сообщения AIVDM (5,24) должны быть перенесены согласно таблице мапинга  (см. Таблицу  $PAISD; Note: поле IMO Number отсутствует в  AIVDM (24) )
@@ -1303,77 +1228,173 @@
 2) В логах КД выявить сообщение об ошибке</t>
   </si>
   <si>
-    <t>- MessageID(uint): AIS message number.  Must be 18 (field automatically set to "18")</t>
-  </si>
-  <si>
-    <t>- RepeatIndicator(uint): Indicated how many times a message has been repeated</t>
-  </si>
-  <si>
-    <t>- UserID(uint): Unique ship identification number (MMSI)</t>
-  </si>
-  <si>
-    <t>- Reserved1(uint): Reseverd for definition by a compentent regional or local authority.  Should be set to zero. (field automatically set to "0")</t>
-  </si>
-  <si>
-    <t>- SOG(udecimal): Speed over ground</t>
-  </si>
-  <si>
-    <t>- PositionAccuracy(uint): Accuracy of positioning fixes</t>
-  </si>
-  <si>
-    <t>- longitude(decimal): Location of the vessel  East West location</t>
-  </si>
-  <si>
-    <t>- latitude(decimal): Location of the vessel  North South location</t>
-  </si>
-  <si>
-    <t>- COG(udecimal): Course over ground</t>
-  </si>
-  <si>
-    <t>- TrueHeading(uint): True heading (relative to true North)</t>
-  </si>
-  <si>
-    <t>- TimeStamp(uint): UTC second when the report was generated</t>
-  </si>
-  <si>
-    <t>- Spare(uint): Not used.  Should be set to zero. (field automatically set to "0")</t>
-  </si>
-  <si>
-    <t>- cs_unit(bool): Does this unit do Carrier Sense?</t>
-  </si>
-  <si>
-    <t>- display_flag(bool): Does this class B unit have an integrated display?</t>
-  </si>
-  <si>
-    <t>- dsc_flag(bool): Does it have dedicated or time-shared DSC radio function?</t>
-  </si>
-  <si>
-    <t>- band_flag(bool): How flexible is the freq handling of the unit?</t>
-  </si>
-  <si>
-    <t>- msg22_flag(bool): Can the unit handle msg 22?</t>
-  </si>
-  <si>
-    <t>- mode_flag(bool): Assigned mode wrt to VDL slots</t>
-  </si>
-  <si>
-    <t>- RAIM(bool): Receiver autonomous integrity monitoring flag</t>
-  </si>
-  <si>
-    <t>- CommStateSelector(uint): SOTDMA or ITDMA</t>
-  </si>
-  <si>
-    <t>- CommState(uint): Not decoded by this software yet</t>
-  </si>
-  <si>
-    <t>AIS LIB FILELDS</t>
+    <t xml:space="preserve">(1) xxxxxxx </t>
+  </si>
+  <si>
+    <t>(2) llll.ll</t>
+  </si>
+  <si>
+    <t>(3) a</t>
+  </si>
+  <si>
+    <t>(4) yyyyy.y</t>
+  </si>
+  <si>
+    <t>(5) a</t>
+  </si>
+  <si>
+    <t>(6) x.x</t>
+  </si>
+  <si>
+    <t>(7) x.x</t>
+  </si>
+  <si>
+    <t>(8) x.x</t>
+  </si>
+  <si>
+    <t>(10) *hh</t>
+  </si>
+  <si>
+    <t>(1) -  идентификатор сопровождаемого АИС суднав МПС (MMSI)</t>
+  </si>
+  <si>
+    <t>(2) -  широта</t>
+  </si>
+  <si>
+    <t>(3) -  признак полушария "N","S"</t>
+  </si>
+  <si>
+    <t>(4) -  долгота</t>
+  </si>
+  <si>
+    <t>(5) -  признак полушария"E","W"</t>
+  </si>
+  <si>
+    <t>(6) -  скорость судна относительно грунта в узлах</t>
+  </si>
+  <si>
+    <t>(7) -  путевой угол судна в градусах</t>
+  </si>
+  <si>
+    <t>(8) -  курс судна в градусах (истинный)</t>
+  </si>
+  <si>
+    <t>(9) -  время получения данных (UTC)</t>
+  </si>
+  <si>
+    <t>(10) - контрольная сумма предложения</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">AIVDM Field: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MMSI</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">AIVDM Field: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Longitude</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">AIVDM Field: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Latitude</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">AIVDM Field: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Speed Over Ground(SOG)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">AIVDM Field: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>True Heading (HDG)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">AIVDM Field: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Course Over Ground (COG)</t>
+    </r>
+  </si>
+  <si>
+    <t>Field: Vessel Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1463,13 +1484,8 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Fira Code"/>
-    </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1518,8 +1534,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1566,12 +1600,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1697,18 +1779,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1742,17 +1812,11 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1762,8 +1826,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2169,10 +2269,10 @@
   <dimension ref="A2:H15"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A9" sqref="A9:H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="1"/>
     <col min="2" max="2" width="47" style="1" customWidth="1"/>
@@ -2185,291 +2285,291 @@
     <col min="9" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8">
-      <c r="A2" s="54" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="54" t="s">
-        <v>327</v>
-      </c>
-      <c r="C2" s="54" t="s">
+      <c r="B2" s="50" t="s">
+        <v>309</v>
+      </c>
+      <c r="C2" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="55" t="s">
+      <c r="D2" s="51" t="s">
         <v>46</v>
       </c>
-      <c r="E2" s="54" t="s">
+      <c r="E2" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="54" t="s">
+      <c r="F2" s="50" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="54" t="s">
+      <c r="G2" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="54" t="s">
+      <c r="H2" s="50" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="159.5">
+    <row r="3" spans="1:8" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A3" s="31">
         <v>1</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>333</v>
+        <v>315</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>335</v>
+        <v>317</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>329</v>
+        <v>311</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>330</v>
+        <v>312</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>340</v>
+        <v>322</v>
       </c>
       <c r="G3" s="33"/>
       <c r="H3" s="34"/>
     </row>
-    <row r="4" spans="1:8" ht="87">
+    <row r="4" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A4" s="31">
         <v>2</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>333</v>
+        <v>315</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>336</v>
+        <v>318</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>328</v>
+        <v>310</v>
       </c>
       <c r="E4" s="33" t="s">
-        <v>331</v>
+        <v>313</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>339</v>
+        <v>321</v>
       </c>
       <c r="G4" s="33"/>
       <c r="H4" s="34"/>
     </row>
-    <row r="5" spans="1:8" ht="58">
+    <row r="5" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="31">
         <v>3</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>333</v>
+        <v>315</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>369</v>
+        <v>344</v>
       </c>
       <c r="D5" s="31"/>
       <c r="E5" s="33" t="s">
-        <v>370</v>
+        <v>345</v>
       </c>
       <c r="F5" s="33" t="s">
-        <v>371</v>
+        <v>346</v>
       </c>
       <c r="G5" s="33"/>
       <c r="H5" s="34"/>
     </row>
-    <row r="6" spans="1:8" ht="58">
+    <row r="6" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="31">
         <v>4</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>333</v>
+        <v>315</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>372</v>
+        <v>347</v>
       </c>
       <c r="D6" s="31"/>
       <c r="E6" s="33" t="s">
-        <v>374</v>
+        <v>349</v>
       </c>
       <c r="F6" s="33" t="s">
-        <v>373</v>
+        <v>348</v>
       </c>
       <c r="G6" s="33"/>
       <c r="H6" s="34"/>
     </row>
-    <row r="7" spans="1:8" ht="87">
+    <row r="7" spans="1:8" ht="87" x14ac:dyDescent="0.35">
       <c r="A7" s="31">
         <v>5</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>333</v>
+        <v>315</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>336</v>
+        <v>318</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>328</v>
+        <v>310</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>331</v>
+        <v>313</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>339</v>
+        <v>321</v>
       </c>
       <c r="G7" s="33"/>
       <c r="H7" s="34"/>
     </row>
-    <row r="8" spans="1:8" ht="72.5">
+    <row r="8" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A8" s="31">
         <v>6</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>333</v>
+        <v>315</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>332</v>
+        <v>314</v>
       </c>
       <c r="D8" s="31"/>
       <c r="E8" s="33" t="s">
-        <v>367</v>
+        <v>342</v>
       </c>
       <c r="F8" s="33" t="s">
-        <v>341</v>
+        <v>323</v>
       </c>
       <c r="G8" s="33"/>
       <c r="H8" s="34"/>
     </row>
-    <row r="9" spans="1:8" ht="58">
-      <c r="A9" s="54">
+    <row r="9" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A9" s="50">
         <v>7</v>
       </c>
-      <c r="B9" s="54" t="s">
-        <v>334</v>
-      </c>
-      <c r="C9" s="56" t="s">
+      <c r="B9" s="50" t="s">
+        <v>316</v>
+      </c>
+      <c r="C9" s="52" t="s">
+        <v>319</v>
+      </c>
+      <c r="D9" s="50"/>
+      <c r="E9" s="53" t="s">
+        <v>320</v>
+      </c>
+      <c r="F9" s="53" t="s">
+        <v>324</v>
+      </c>
+      <c r="G9" s="53"/>
+      <c r="H9" s="54"/>
+    </row>
+    <row r="10" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A10" s="50">
+        <v>8</v>
+      </c>
+      <c r="B10" s="50" t="s">
+        <v>316</v>
+      </c>
+      <c r="C10" s="52" t="s">
+        <v>328</v>
+      </c>
+      <c r="D10" s="50"/>
+      <c r="E10" s="53" t="s">
+        <v>340</v>
+      </c>
+      <c r="F10" s="53" t="s">
+        <v>330</v>
+      </c>
+      <c r="G10" s="53"/>
+      <c r="H10" s="54"/>
+    </row>
+    <row r="11" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="50">
+        <v>9</v>
+      </c>
+      <c r="B11" s="50" t="s">
+        <v>316</v>
+      </c>
+      <c r="C11" s="52" t="s">
+        <v>329</v>
+      </c>
+      <c r="D11" s="50"/>
+      <c r="E11" s="53" t="s">
+        <v>341</v>
+      </c>
+      <c r="F11" s="53" t="s">
         <v>337</v>
       </c>
-      <c r="D9" s="54"/>
-      <c r="E9" s="57" t="s">
+      <c r="G11" s="53"/>
+      <c r="H11" s="54"/>
+    </row>
+    <row r="12" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A12" s="50">
+        <v>10</v>
+      </c>
+      <c r="B12" s="50" t="s">
+        <v>316</v>
+      </c>
+      <c r="C12" s="52" t="s">
         <v>338</v>
       </c>
-      <c r="F9" s="57" t="s">
-        <v>342</v>
-      </c>
-      <c r="G9" s="57"/>
-      <c r="H9" s="58"/>
-    </row>
-    <row r="10" spans="1:8" ht="58">
-      <c r="A10" s="54">
-        <v>8</v>
-      </c>
-      <c r="B10" s="54" t="s">
-        <v>334</v>
-      </c>
-      <c r="C10" s="56" t="s">
+      <c r="D12" s="54"/>
+      <c r="E12" s="53" t="s">
+        <v>343</v>
+      </c>
+      <c r="F12" s="53" t="s">
+        <v>350</v>
+      </c>
+      <c r="G12" s="54"/>
+      <c r="H12" s="54"/>
+    </row>
+    <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="50">
+        <v>11</v>
+      </c>
+      <c r="B13" s="50" t="s">
+        <v>316</v>
+      </c>
+      <c r="C13" s="52"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="53" t="s">
+        <v>343</v>
+      </c>
+      <c r="F13" s="53" t="s">
+        <v>351</v>
+      </c>
+      <c r="G13" s="54"/>
+      <c r="H13" s="54"/>
+    </row>
+    <row r="14" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="50">
+        <v>12</v>
+      </c>
+      <c r="B14" s="50" t="s">
+        <v>316</v>
+      </c>
+      <c r="C14" s="52"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="53" t="s">
         <v>352</v>
       </c>
-      <c r="D10" s="54"/>
-      <c r="E10" s="57" t="s">
-        <v>365</v>
-      </c>
-      <c r="F10" s="57" t="s">
-        <v>354</v>
-      </c>
-      <c r="G10" s="57"/>
-      <c r="H10" s="58"/>
-    </row>
-    <row r="11" spans="1:8" ht="72.5">
-      <c r="A11" s="54">
-        <v>9</v>
-      </c>
-      <c r="B11" s="54" t="s">
-        <v>334</v>
-      </c>
-      <c r="C11" s="56" t="s">
-        <v>353</v>
-      </c>
-      <c r="D11" s="54"/>
-      <c r="E11" s="57" t="s">
-        <v>366</v>
-      </c>
-      <c r="F11" s="57" t="s">
-        <v>362</v>
-      </c>
-      <c r="G11" s="57"/>
-      <c r="H11" s="58"/>
-    </row>
-    <row r="12" spans="1:8" ht="58">
-      <c r="A12" s="54">
-        <v>10</v>
-      </c>
-      <c r="B12" s="54" t="s">
-        <v>334</v>
-      </c>
-      <c r="C12" s="56" t="s">
-        <v>363</v>
-      </c>
-      <c r="D12" s="58"/>
-      <c r="E12" s="57" t="s">
-        <v>368</v>
-      </c>
-      <c r="F12" s="57" t="s">
-        <v>375</v>
-      </c>
-      <c r="G12" s="58"/>
-      <c r="H12" s="58"/>
-    </row>
-    <row r="13" spans="1:8" ht="43.5">
-      <c r="A13" s="54">
-        <v>11</v>
-      </c>
-      <c r="B13" s="54" t="s">
-        <v>334</v>
-      </c>
-      <c r="C13" s="56"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="57" t="s">
-        <v>368</v>
-      </c>
-      <c r="F13" s="57" t="s">
-        <v>376</v>
-      </c>
-      <c r="G13" s="58"/>
-      <c r="H13" s="58"/>
-    </row>
-    <row r="14" spans="1:8" ht="43.5">
-      <c r="A14" s="54">
-        <v>12</v>
-      </c>
-      <c r="B14" s="54" t="s">
-        <v>334</v>
-      </c>
-      <c r="C14" s="56"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="57" t="s">
-        <v>377</v>
-      </c>
-      <c r="F14" s="57" t="s">
-        <v>375</v>
-      </c>
-      <c r="G14" s="58"/>
-      <c r="H14" s="58"/>
-    </row>
-    <row r="15" spans="1:8" ht="43.5">
-      <c r="A15" s="54">
+      <c r="F14" s="53" t="s">
+        <v>350</v>
+      </c>
+      <c r="G14" s="54"/>
+      <c r="H14" s="54"/>
+    </row>
+    <row r="15" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="50">
         <v>13</v>
       </c>
-      <c r="B15" s="54" t="s">
-        <v>334</v>
-      </c>
-      <c r="C15" s="56"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="57" t="s">
-        <v>377</v>
-      </c>
-      <c r="F15" s="57" t="s">
-        <v>376</v>
-      </c>
-      <c r="G15" s="58"/>
-      <c r="H15" s="58"/>
+      <c r="B15" s="50" t="s">
+        <v>316</v>
+      </c>
+      <c r="C15" s="52"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="53" t="s">
+        <v>352</v>
+      </c>
+      <c r="F15" s="53" t="s">
+        <v>351</v>
+      </c>
+      <c r="G15" s="54"/>
+      <c r="H15" s="54"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2485,7 +2585,7 @@
       <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="31.453125" customWidth="1"/>
     <col min="2" max="2" width="37.90625" customWidth="1"/>
@@ -2495,7 +2595,7 @@
     <col min="6" max="6" width="25.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -2503,7 +2603,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
@@ -2511,7 +2611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
@@ -2519,7 +2619,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>7</v>
       </c>
@@ -2539,7 +2639,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -2547,7 +2647,7 @@
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>7</v>
       </c>
@@ -2555,7 +2655,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>8</v>
       </c>
@@ -2563,7 +2663,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>9</v>
       </c>
@@ -2571,7 +2671,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>10</v>
       </c>
@@ -2579,7 +2679,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>11</v>
       </c>
@@ -2587,7 +2687,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>12</v>
       </c>
@@ -2595,25 +2695,25 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="10"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="10"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="10"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>22</v>
       </c>
@@ -2621,7 +2721,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
         <v>24</v>
       </c>
@@ -2629,7 +2729,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
         <v>26</v>
       </c>
@@ -2637,12 +2737,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>7</v>
       </c>
@@ -2663,7 +2763,7 @@
       </c>
       <c r="G22" s="14"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="8">
         <v>1</v>
       </c>
@@ -2678,7 +2778,7 @@
       <c r="F23" s="8"/>
       <c r="G23" s="14"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="14">
         <v>2</v>
       </c>
@@ -2693,7 +2793,7 @@
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="14">
         <v>3</v>
       </c>
@@ -2712,7 +2812,7 @@
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="14"/>
       <c r="B26" s="16" t="s">
         <v>35</v>
@@ -2733,7 +2833,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="14"/>
       <c r="B27" s="16" t="s">
         <v>39</v>
@@ -2750,16 +2850,16 @@
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B28" s="16"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B29" s="16"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B30" s="16"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B31" s="16"/>
     </row>
   </sheetData>
@@ -2776,143 +2876,157 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.90625" style="2" customWidth="1"/>
     <col min="2" max="2" width="32.36328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="46.1796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.453125" style="4" customWidth="1"/>
     <col min="5" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="43" customFormat="1" ht="15.5">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:4" s="43" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="63" t="s">
         <v>138</v>
       </c>
-      <c r="C1" s="47" t="s">
-        <v>346</v>
-      </c>
-      <c r="D1" s="43" t="s">
+      <c r="B1" s="64"/>
+      <c r="C1" s="62" t="s">
+        <v>326</v>
+      </c>
+      <c r="D1" s="67" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="69" t="s">
+        <v>353</v>
+      </c>
+      <c r="B2" s="68" t="s">
+        <v>362</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>372</v>
+      </c>
+      <c r="D2" s="66"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="69" t="s">
+        <v>354</v>
+      </c>
+      <c r="B3" s="68" t="s">
+        <v>363</v>
+      </c>
+      <c r="C3" s="72" t="s">
+        <v>373</v>
+      </c>
+      <c r="D3" s="66"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="70" t="s">
+        <v>355</v>
+      </c>
+      <c r="B4" s="68" t="s">
+        <v>364</v>
+      </c>
+      <c r="C4" s="73" t="s">
+        <v>327</v>
+      </c>
+      <c r="D4" s="66"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="69" t="s">
+        <v>356</v>
+      </c>
+      <c r="B5" s="68" t="s">
+        <v>365</v>
+      </c>
+      <c r="C5" s="72" t="s">
+        <v>374</v>
+      </c>
+      <c r="D5" s="66"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="69" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" s="4" customFormat="1" ht="43.5">
-      <c r="A2" s="44" t="s">
-        <v>139</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="44" t="s">
-        <v>140</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="45" t="s">
-        <v>141</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="44" t="s">
-        <v>142</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="44" t="s">
-        <v>143</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="29">
-      <c r="A7" s="44" t="s">
-        <v>144</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="44" t="s">
+      <c r="B6" s="68" t="s">
+        <v>366</v>
+      </c>
+      <c r="C6" s="73" t="s">
+        <v>327</v>
+      </c>
+      <c r="D6" s="66"/>
+    </row>
+    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="69" t="s">
+        <v>358</v>
+      </c>
+      <c r="B7" s="68" t="s">
+        <v>367</v>
+      </c>
+      <c r="C7" s="72" t="s">
+        <v>375</v>
+      </c>
+      <c r="D7" s="66" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="69" t="s">
+        <v>359</v>
+      </c>
+      <c r="B8" s="68" t="s">
+        <v>368</v>
+      </c>
+      <c r="C8" s="72" t="s">
+        <v>376</v>
+      </c>
+      <c r="D8" s="66"/>
+    </row>
+    <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="69" t="s">
+        <v>360</v>
+      </c>
+      <c r="B9" s="68" t="s">
+        <v>369</v>
+      </c>
+      <c r="C9" s="72" t="s">
+        <v>377</v>
+      </c>
+      <c r="D9" s="66"/>
+    </row>
+    <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="69" t="s">
+        <v>325</v>
+      </c>
+      <c r="B10" s="68" t="s">
+        <v>370</v>
+      </c>
+      <c r="C10" s="73" t="s">
+        <v>327</v>
+      </c>
+      <c r="D10" s="66"/>
+    </row>
+    <row r="11" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="69" t="s">
+        <v>361</v>
+      </c>
+      <c r="B11" s="68" t="s">
+        <v>371</v>
+      </c>
+      <c r="C11" s="61"/>
+      <c r="D11" s="66"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="71" t="s">
         <v>145</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="29">
-      <c r="A9" s="44" t="s">
-        <v>146</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="44" t="s">
-        <v>343</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="29">
-      <c r="A11" s="44" t="s">
-        <v>344</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="2" t="s">
-        <v>163</v>
-      </c>
+      <c r="B12" s="65"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="66"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2925,46 +3039,46 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.26953125" style="28" customWidth="1"/>
+    <col min="1" max="1" width="23.90625" style="28" customWidth="1"/>
     <col min="2" max="2" width="8.7265625" style="3"/>
     <col min="3" max="3" width="23.6328125" style="3" customWidth="1"/>
     <col min="4" max="4" width="21" style="3" customWidth="1"/>
     <col min="5" max="5" width="8.7265625" style="3"/>
-    <col min="6" max="6" width="44.81640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="60.7265625" style="3" customWidth="1"/>
     <col min="7" max="7" width="8.7265625" style="3"/>
     <col min="8" max="8" width="10.6328125" style="3" customWidth="1"/>
     <col min="9" max="9" width="50.08984375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="55" customHeight="1">
-      <c r="A1" s="61" t="s">
-        <v>169</v>
-      </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-    </row>
-    <row r="2" spans="1:9" ht="16" thickBot="1">
-      <c r="A2" s="63" t="s">
-        <v>170</v>
-      </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
+    <row r="1" spans="1:9" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="55" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+    </row>
+    <row r="2" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="57" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
       <c r="H2" s="24" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="18" thickBot="1">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="25" t="s">
         <v>49</v>
       </c>
@@ -2980,17 +3094,17 @@
       <c r="E3" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="59" t="s">
+      <c r="F3" s="20" t="s">
         <v>54</v>
       </c>
       <c r="H3" s="18">
         <v>0</v>
       </c>
       <c r="I3" s="18" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="18" thickBot="1">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="26" t="s">
         <v>55</v>
       </c>
@@ -3006,17 +3120,17 @@
       <c r="E4" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="60" t="s">
-        <v>173</v>
+      <c r="F4" s="18" t="s">
+        <v>155</v>
       </c>
       <c r="H4" s="18">
         <v>1</v>
       </c>
       <c r="I4" s="18" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="18" thickBot="1">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="26">
         <v>43287</v>
       </c>
@@ -3032,17 +3146,17 @@
       <c r="E5" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="60" t="s">
-        <v>175</v>
+      <c r="F5" s="18" t="s">
+        <v>157</v>
       </c>
       <c r="H5" s="18">
         <v>2</v>
       </c>
       <c r="I5" s="18" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="18" thickBot="1">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="26">
         <v>13728</v>
       </c>
@@ -3058,77 +3172,77 @@
       <c r="E6" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="60" t="s">
+      <c r="F6" s="18" t="s">
         <v>67</v>
       </c>
       <c r="H6" s="18">
         <v>3</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="18" thickBot="1">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="26" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
       <c r="B7" s="18">
         <v>4</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="F7" s="60" t="s">
-        <v>182</v>
+        <v>163</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>164</v>
       </c>
       <c r="H7" s="18">
         <v>4</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="35.5" thickBot="1">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="26" t="s">
-        <v>184</v>
+        <v>166</v>
       </c>
       <c r="B8" s="18">
         <v>8</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="F8" s="60" t="s">
+        <v>169</v>
+      </c>
+      <c r="F8" s="18" t="s">
         <v>81</v>
       </c>
       <c r="H8" s="18">
         <v>5</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="35.5" thickBot="1">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="26" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="B9" s="18">
         <v>10</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>75</v>
@@ -3136,19 +3250,19 @@
       <c r="E9" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="F9" s="60" t="s">
+      <c r="F9" s="18" t="s">
         <v>81</v>
       </c>
       <c r="H9" s="18">
         <v>6</v>
       </c>
       <c r="I9" s="18" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="18" thickBot="1">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="26" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="B10" s="18">
         <v>1</v>
@@ -3162,19 +3276,19 @@
       <c r="E10" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="F10" s="60" t="s">
+      <c r="F10" s="18" t="s">
         <v>81</v>
       </c>
       <c r="H10" s="18">
         <v>7</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="18" thickBot="1">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="26" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="B11" s="18">
         <v>28</v>
@@ -3188,19 +3302,19 @@
       <c r="E11" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="F11" s="60" t="s">
-        <v>195</v>
+      <c r="F11" s="18" t="s">
+        <v>177</v>
       </c>
       <c r="H11" s="18">
         <v>8</v>
       </c>
       <c r="I11" s="18" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="35.5" thickBot="1">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="26" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="B12" s="18">
         <v>27</v>
@@ -3214,25 +3328,25 @@
       <c r="E12" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="F12" s="60" t="s">
-        <v>195</v>
+      <c r="F12" s="18" t="s">
+        <v>177</v>
       </c>
       <c r="H12" s="18">
         <v>9</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="35.5" thickBot="1">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="26" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="B13" s="18">
         <v>12</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>200</v>
+        <v>182</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>92</v>
@@ -3240,25 +3354,25 @@
       <c r="E13" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="F13" s="60" t="s">
-        <v>201</v>
+      <c r="F13" s="18" t="s">
+        <v>183</v>
       </c>
       <c r="H13" s="18">
         <v>10</v>
       </c>
       <c r="I13" s="18" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="35.5" thickBot="1">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="26" t="s">
-        <v>203</v>
+        <v>185</v>
       </c>
       <c r="B14" s="18">
         <v>9</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>204</v>
+        <v>186</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>96</v>
@@ -3266,19 +3380,19 @@
       <c r="E14" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="60" t="s">
-        <v>205</v>
+      <c r="F14" s="18" t="s">
+        <v>187</v>
       </c>
       <c r="H14" s="18">
         <v>11</v>
       </c>
       <c r="I14" s="18" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="18" thickBot="1">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="26" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="B15" s="18">
         <v>6</v>
@@ -3292,69 +3406,69 @@
       <c r="E15" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="F15" s="60" t="s">
-        <v>208</v>
+      <c r="F15" s="18" t="s">
+        <v>190</v>
       </c>
       <c r="H15" s="18">
         <v>12</v>
       </c>
       <c r="I15" s="18" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="35.5" thickBot="1">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="26" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="B16" s="18">
         <v>2</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="F16" s="60" t="s">
-        <v>212</v>
+        <v>163</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>194</v>
       </c>
       <c r="H16" s="18">
         <v>13</v>
       </c>
       <c r="I16" s="18" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="18" thickBot="1">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="26" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="B17" s="18">
         <v>3</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="D17" s="27"/>
       <c r="E17" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="F17" s="60" t="s">
+      <c r="F17" s="18" t="s">
         <v>72</v>
       </c>
       <c r="H17" s="18">
         <v>14</v>
       </c>
       <c r="I17" s="18" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="18" thickBot="1">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="26" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="B18" s="18">
         <v>1</v>
@@ -3368,19 +3482,19 @@
       <c r="E18" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="F18" s="60" t="s">
+      <c r="F18" s="18" t="s">
         <v>81</v>
       </c>
       <c r="H18" s="18">
         <v>15</v>
       </c>
       <c r="I18" s="18" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="18" thickBot="1">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="26" t="s">
-        <v>218</v>
+        <v>200</v>
       </c>
       <c r="B19" s="18">
         <v>19</v>
@@ -3394,7 +3508,7 @@
       <c r="E19" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="F19" s="60" t="s">
+      <c r="F19" s="18" t="s">
         <v>81</v>
       </c>
     </row>
@@ -3410,42 +3524,40 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="26.36328125" style="23" customWidth="1"/>
     <col min="2" max="2" width="8.7265625" style="23"/>
     <col min="3" max="3" width="28.1796875" style="23" customWidth="1"/>
     <col min="4" max="5" width="8.7265625" style="23"/>
     <col min="6" max="6" width="54.1796875" style="23" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" style="19"/>
-    <col min="8" max="8" width="158.54296875" style="19" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="19"/>
+    <col min="7" max="16384" width="8.7265625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1">
-      <c r="A1" s="64" t="s">
+    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="58" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-    </row>
-    <row r="2" spans="1:13" ht="35.5" thickBot="1">
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+    </row>
+    <row r="2" spans="1:13" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="20" t="s">
         <v>49</v>
       </c>
@@ -3464,11 +3576,8 @@
       <c r="F2" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="H2" s="19" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="18" thickBot="1">
+    </row>
+    <row r="3" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="18" t="s">
         <v>55</v>
       </c>
@@ -3487,11 +3596,8 @@
       <c r="F3" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="H3" s="67" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="18" thickBot="1">
+    </row>
+    <row r="4" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="21" t="s">
         <v>60</v>
       </c>
@@ -3510,11 +3616,8 @@
       <c r="F4" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="H4" s="67" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="18" thickBot="1">
+    </row>
+    <row r="5" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="21" t="s">
         <v>64</v>
       </c>
@@ -3533,11 +3636,8 @@
       <c r="F5" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="H5" s="67" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="35.5" thickBot="1">
+    </row>
+    <row r="6" spans="1:13" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="18" t="s">
         <v>68</v>
       </c>
@@ -3556,11 +3656,8 @@
       <c r="F6" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="H6" s="67" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="18" thickBot="1">
+    </row>
+    <row r="7" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="18" t="s">
         <v>73</v>
       </c>
@@ -3579,11 +3676,8 @@
       <c r="F7" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="H7" s="67" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="35.5" thickBot="1">
+    </row>
+    <row r="8" spans="1:13" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="18" t="s">
         <v>78</v>
       </c>
@@ -3602,11 +3696,8 @@
       <c r="F8" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="H8" s="67" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="18" thickBot="1">
+    </row>
+    <row r="9" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="18" t="s">
         <v>82</v>
       </c>
@@ -3625,11 +3716,8 @@
       <c r="F9" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="H9" s="67" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="18" thickBot="1">
+    </row>
+    <row r="10" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="18" t="s">
         <v>87</v>
       </c>
@@ -3648,11 +3736,8 @@
       <c r="F10" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="H10" s="67" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="18" thickBot="1">
+    </row>
+    <row r="11" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="18" t="s">
         <v>90</v>
       </c>
@@ -3671,11 +3756,8 @@
       <c r="F11" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="H11" s="67" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="35.5" thickBot="1">
+    </row>
+    <row r="12" spans="1:13" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="18" t="s">
         <v>94</v>
       </c>
@@ -3694,11 +3776,8 @@
       <c r="F12" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="H12" s="67" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="35.5" thickBot="1">
+    </row>
+    <row r="13" spans="1:13" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="18" t="s">
         <v>98</v>
       </c>
@@ -3717,11 +3796,8 @@
       <c r="F13" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="H13" s="67" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="35.5" thickBot="1">
+    </row>
+    <row r="14" spans="1:13" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="18" t="s">
         <v>102</v>
       </c>
@@ -3740,11 +3816,8 @@
       <c r="F14" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="H14" s="67" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="35.5" thickBot="1">
+    </row>
+    <row r="15" spans="1:13" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="18" t="s">
         <v>106</v>
       </c>
@@ -3763,11 +3836,8 @@
       <c r="F15" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="H15" s="67" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="35.5" thickBot="1">
+    </row>
+    <row r="16" spans="1:13" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="18" t="s">
         <v>110</v>
       </c>
@@ -3786,11 +3856,8 @@
       <c r="F16" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="H16" s="67" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="35.5" thickBot="1">
+    </row>
+    <row r="17" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="18" t="s">
         <v>114</v>
       </c>
@@ -3809,11 +3876,8 @@
       <c r="F17" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="H17" s="67" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="53" thickBot="1">
+    </row>
+    <row r="18" spans="1:6" ht="53" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="18" t="s">
         <v>118</v>
       </c>
@@ -3832,11 +3896,8 @@
       <c r="F18" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="H18" s="67" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="35.5" thickBot="1">
+    </row>
+    <row r="19" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="18" t="s">
         <v>122</v>
       </c>
@@ -3855,11 +3916,8 @@
       <c r="F19" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="H19" s="67" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="35.5" thickBot="1">
+    </row>
+    <row r="20" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="18" t="s">
         <v>126</v>
       </c>
@@ -3878,11 +3936,8 @@
       <c r="F20" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="H20" s="67" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="18" thickBot="1">
+    </row>
+    <row r="21" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="18" t="s">
         <v>130</v>
       </c>
@@ -3901,11 +3956,8 @@
       <c r="F21" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="H21" s="67" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="18" thickBot="1">
+    </row>
+    <row r="22" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="18" t="s">
         <v>134</v>
       </c>
@@ -3923,14 +3975,6 @@
       </c>
       <c r="F22" s="22" t="s">
         <v>137</v>
-      </c>
-      <c r="H22" s="67" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="H23" s="67" t="s">
-        <v>398</v>
       </c>
     </row>
   </sheetData>
@@ -3941,7 +3985,6 @@
     <hyperlink ref="F22" r:id="rId1" location="IALA" display="http://catb.org/gpsd/AIVDM.html - IALA"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3949,13 +3992,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="48"/>
+    <col min="1" max="1" width="8.7265625" style="44"/>
     <col min="2" max="2" width="17.90625" style="4" customWidth="1"/>
     <col min="3" max="3" width="22.1796875" style="4" customWidth="1"/>
     <col min="4" max="4" width="21.453125" style="4" customWidth="1"/>
@@ -3963,79 +4006,79 @@
     <col min="6" max="16384" width="8.7265625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="51" t="s">
-        <v>157</v>
-      </c>
-      <c r="B1" s="50"/>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="47" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="46"/>
       <c r="C1" s="29" t="s">
-        <v>355</v>
-      </c>
-      <c r="D1" s="53" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="58">
-      <c r="A2" s="49" t="s">
-        <v>158</v>
-      </c>
-      <c r="B2" s="50" t="s">
-        <v>164</v>
+        <v>331</v>
+      </c>
+      <c r="D1" s="49" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A2" s="45" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="46" t="s">
+        <v>146</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="58">
-      <c r="A3" s="49" t="s">
-        <v>159</v>
-      </c>
-      <c r="B3" s="50" t="s">
-        <v>165</v>
+        <v>332</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A3" s="45" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>147</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>358</v>
-      </c>
-      <c r="D3" s="52" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="72.5">
-      <c r="A4" s="49" t="s">
-        <v>160</v>
-      </c>
-      <c r="B4" s="50" t="s">
-        <v>166</v>
+        <v>334</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4" s="46" t="s">
+        <v>148</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="72.5">
-      <c r="A5" s="49" t="s">
-        <v>161</v>
-      </c>
-      <c r="B5" s="50" t="s">
-        <v>167</v>
+        <v>336</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="45" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" s="46" t="s">
+        <v>149</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="43.5">
-      <c r="A6" s="49" t="s">
-        <v>162</v>
-      </c>
-      <c r="B6" s="50" t="s">
-        <v>168</v>
+        <v>378</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="45" t="s">
+        <v>144</v>
+      </c>
+      <c r="B6" s="46" t="s">
+        <v>150</v>
       </c>
       <c r="C6" s="30"/>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="49" t="s">
-        <v>163</v>
-      </c>
-      <c r="B7" s="50"/>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="B7" s="46"/>
       <c r="C7" s="30"/>
     </row>
   </sheetData>
@@ -4052,7 +4095,7 @@
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.7265625" style="23" customWidth="1"/>
     <col min="2" max="2" width="8.7265625" style="23"/>
@@ -4070,12 +4113,12 @@
     <col min="14" max="16384" width="8.7265625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" customHeight="1" thickBot="1">
+    <row r="1" spans="1:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="23" t="s">
-        <v>291</v>
+        <v>273</v>
       </c>
       <c r="H1" s="41" t="s">
-        <v>219</v>
+        <v>201</v>
       </c>
       <c r="I1" s="41"/>
       <c r="J1" s="41"/>
@@ -4083,7 +4126,7 @@
       <c r="L1" s="41"/>
       <c r="M1" s="41"/>
     </row>
-    <row r="2" spans="1:13" ht="18" thickBot="1">
+    <row r="2" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="36" t="s">
         <v>49</v>
       </c>
@@ -4112,16 +4155,16 @@
         <v>51</v>
       </c>
       <c r="K2" s="36" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="L2" s="36" t="s">
         <v>53</v>
       </c>
       <c r="M2" s="36" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="18" thickBot="1">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="37" t="s">
         <v>55</v>
       </c>
@@ -4138,7 +4181,7 @@
         <v>58</v>
       </c>
       <c r="F3" s="37" t="s">
-        <v>292</v>
+        <v>274</v>
       </c>
       <c r="H3" s="37" t="s">
         <v>55</v>
@@ -4156,10 +4199,10 @@
         <v>58</v>
       </c>
       <c r="M3" s="37" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="18" thickBot="1">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="38" t="s">
         <v>60</v>
       </c>
@@ -4176,7 +4219,7 @@
         <v>58</v>
       </c>
       <c r="F4" s="37" t="s">
-        <v>293</v>
+        <v>275</v>
       </c>
       <c r="H4" s="38" t="s">
         <v>60</v>
@@ -4194,10 +4237,10 @@
         <v>58</v>
       </c>
       <c r="M4" s="37" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="18" thickBot="1">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="38" t="s">
         <v>64</v>
       </c>
@@ -4214,7 +4257,7 @@
         <v>58</v>
       </c>
       <c r="F5" s="37" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
       <c r="H5" s="38" t="s">
         <v>64</v>
@@ -4232,606 +4275,606 @@
         <v>58</v>
       </c>
       <c r="M5" s="37" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="18" thickBot="1">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="37" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="B6" s="37">
         <v>2</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>295</v>
+        <v>277</v>
       </c>
       <c r="E6" s="37" t="s">
         <v>58</v>
       </c>
       <c r="F6" s="37" t="s">
-        <v>296</v>
+        <v>278</v>
       </c>
       <c r="H6" s="37" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="I6" s="37">
         <v>2</v>
       </c>
       <c r="J6" s="37" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="K6" s="37" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="L6" s="37" t="s">
         <v>58</v>
       </c>
       <c r="M6" s="39" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="18" thickBot="1">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="37" t="s">
-        <v>297</v>
+        <v>279</v>
       </c>
       <c r="B7" s="37">
         <v>120</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>238</v>
+        <v>220</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
       <c r="F7" s="37" t="s">
-        <v>298</v>
+        <v>280</v>
       </c>
       <c r="H7" s="37" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="I7" s="37">
         <v>30</v>
       </c>
       <c r="J7" s="42" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="K7" s="37" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="L7" s="37" t="s">
         <v>58</v>
       </c>
       <c r="M7" s="37" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="18" thickBot="1">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="37" t="s">
-        <v>299</v>
+        <v>281</v>
       </c>
       <c r="B8" s="37">
         <v>8</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="D8" s="40"/>
       <c r="E8" s="37" t="s">
         <v>71</v>
       </c>
       <c r="F8" s="37" t="s">
-        <v>300</v>
+        <v>282</v>
       </c>
       <c r="H8" s="37" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="I8" s="37">
         <v>42</v>
       </c>
       <c r="J8" s="42" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="K8" s="37" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="L8" s="37" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
       <c r="M8" s="37" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="18" thickBot="1">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="37" t="s">
-        <v>301</v>
+        <v>283</v>
       </c>
       <c r="B9" s="37">
         <v>8</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>302</v>
+        <v>284</v>
       </c>
       <c r="H9" s="37" t="s">
-        <v>237</v>
+        <v>219</v>
       </c>
       <c r="I9" s="37">
         <v>120</v>
       </c>
       <c r="J9" s="37" t="s">
-        <v>238</v>
+        <v>220</v>
       </c>
       <c r="K9" s="37" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
       <c r="L9" s="37" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
       <c r="M9" s="37" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="18" thickBot="1">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="37" t="s">
-        <v>303</v>
+        <v>285</v>
       </c>
       <c r="B10" s="37">
         <v>18</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>304</v>
+        <v>286</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>305</v>
+        <v>287</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
       <c r="F10" s="37" t="s">
-        <v>306</v>
+        <v>288</v>
       </c>
       <c r="H10" s="37" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
       <c r="I10" s="37">
         <v>8</v>
       </c>
       <c r="J10" s="37" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
       <c r="K10" s="37" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="L10" s="37" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
       <c r="M10" s="37" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="18" thickBot="1">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="37" t="s">
-        <v>307</v>
+        <v>289</v>
       </c>
       <c r="B11" s="37">
         <v>4</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>308</v>
+        <v>290</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>309</v>
+        <v>291</v>
       </c>
       <c r="E11" s="37" t="s">
         <v>58</v>
       </c>
       <c r="F11" s="37" t="s">
-        <v>310</v>
+        <v>292</v>
       </c>
       <c r="H11" s="37" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
       <c r="I11" s="37">
         <v>9</v>
       </c>
       <c r="J11" s="37" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="K11" s="37" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="L11" s="37" t="s">
         <v>58</v>
       </c>
       <c r="M11" s="37" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="18" thickBot="1">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="37" t="s">
-        <v>311</v>
+        <v>293</v>
       </c>
       <c r="B12" s="37">
         <v>20</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>312</v>
+        <v>294</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>313</v>
+        <v>295</v>
       </c>
       <c r="E12" s="37" t="s">
         <v>58</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>310</v>
+        <v>292</v>
       </c>
       <c r="H12" s="37" t="s">
-        <v>249</v>
+        <v>231</v>
       </c>
       <c r="I12" s="37">
         <v>9</v>
       </c>
       <c r="J12" s="37" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="K12" s="37" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="L12" s="37" t="s">
         <v>58</v>
       </c>
       <c r="M12" s="37" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="18" thickBot="1">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="37" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="B13" s="37">
         <v>42</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="D13" s="37" t="s">
+        <v>216</v>
+      </c>
+      <c r="E13" s="37" t="s">
+        <v>217</v>
+      </c>
+      <c r="F13" s="37" t="s">
+        <v>297</v>
+      </c>
+      <c r="H13" s="37" t="s">
         <v>234</v>
-      </c>
-      <c r="E13" s="37" t="s">
-        <v>235</v>
-      </c>
-      <c r="F13" s="37" t="s">
-        <v>315</v>
-      </c>
-      <c r="H13" s="37" t="s">
-        <v>252</v>
       </c>
       <c r="I13" s="37">
         <v>6</v>
       </c>
       <c r="J13" s="37" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
       <c r="K13" s="37" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
       <c r="L13" s="37" t="s">
         <v>58</v>
       </c>
       <c r="M13" s="37" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="18" thickBot="1">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="37" t="s">
-        <v>316</v>
+        <v>298</v>
       </c>
       <c r="B14" s="37">
         <v>9</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="E14" s="37" t="s">
         <v>58</v>
       </c>
       <c r="F14" s="37" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
       <c r="H14" s="37" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
       <c r="I14" s="37">
         <v>6</v>
       </c>
       <c r="J14" s="37" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
       <c r="K14" s="37" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="L14" s="37" t="s">
         <v>58</v>
       </c>
       <c r="M14" s="37" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="18" thickBot="1">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="37" t="s">
-        <v>318</v>
+        <v>300</v>
       </c>
       <c r="B15" s="37">
         <v>9</v>
       </c>
       <c r="C15" s="37" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="E15" s="37" t="s">
         <v>58</v>
       </c>
       <c r="F15" s="37" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
       <c r="H15" s="37" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
       <c r="I15" s="37">
         <v>4</v>
       </c>
       <c r="J15" s="37" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
       <c r="K15" s="37" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
       <c r="L15" s="37" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
       <c r="M15" s="37" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="18" thickBot="1">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="37" t="s">
-        <v>319</v>
+        <v>301</v>
       </c>
       <c r="B16" s="37">
         <v>6</v>
       </c>
       <c r="C16" s="37" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
       <c r="E16" s="37" t="s">
         <v>58</v>
       </c>
       <c r="F16" s="37" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
       <c r="H16" s="37" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
       <c r="I16" s="37">
         <v>4</v>
       </c>
       <c r="J16" s="37" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
       <c r="K16" s="37" t="s">
-        <v>264</v>
+        <v>246</v>
       </c>
       <c r="L16" s="37" t="s">
         <v>58</v>
       </c>
       <c r="M16" s="37" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="18" thickBot="1">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="37" t="s">
-        <v>320</v>
+        <v>302</v>
       </c>
       <c r="B17" s="37">
         <v>6</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
       <c r="D17" s="37" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="E17" s="37" t="s">
         <v>58</v>
       </c>
       <c r="F17" s="37" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
       <c r="H17" s="37" t="s">
-        <v>266</v>
+        <v>248</v>
       </c>
       <c r="I17" s="37">
         <v>5</v>
       </c>
       <c r="J17" s="37" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="K17" s="37" t="s">
-        <v>268</v>
+        <v>250</v>
       </c>
       <c r="L17" s="37" t="s">
         <v>58</v>
       </c>
       <c r="M17" s="37" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="18" thickBot="1">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="37" t="s">
-        <v>321</v>
+        <v>303</v>
       </c>
       <c r="B18" s="37">
         <v>30</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>322</v>
+        <v>304</v>
       </c>
       <c r="D18" s="37" t="s">
-        <v>323</v>
+        <v>305</v>
       </c>
       <c r="E18" s="37" t="s">
         <v>58</v>
       </c>
       <c r="F18" s="37" t="s">
-        <v>324</v>
+        <v>306</v>
       </c>
       <c r="H18" s="37" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="I18" s="37">
         <v>5</v>
       </c>
       <c r="J18" s="37" t="s">
-        <v>271</v>
+        <v>253</v>
       </c>
       <c r="K18" s="37" t="s">
-        <v>272</v>
+        <v>254</v>
       </c>
       <c r="L18" s="37" t="s">
         <v>58</v>
       </c>
       <c r="M18" s="37" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="18" thickBot="1">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="37" t="s">
-        <v>325</v>
+        <v>307</v>
       </c>
       <c r="B19" s="37">
         <v>6</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="D19" s="40"/>
       <c r="E19" s="37" t="s">
         <v>71</v>
       </c>
       <c r="F19" s="37" t="s">
-        <v>326</v>
+        <v>308</v>
       </c>
       <c r="H19" s="37" t="s">
-        <v>274</v>
+        <v>256</v>
       </c>
       <c r="I19" s="37">
         <v>6</v>
       </c>
       <c r="J19" s="37" t="s">
-        <v>275</v>
+        <v>257</v>
       </c>
       <c r="K19" s="37" t="s">
-        <v>276</v>
+        <v>258</v>
       </c>
       <c r="L19" s="37" t="s">
         <v>58</v>
       </c>
       <c r="M19" s="37" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="18" thickBot="1">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="H20" s="37" t="s">
-        <v>278</v>
+        <v>260</v>
       </c>
       <c r="I20" s="37">
         <v>8</v>
       </c>
       <c r="J20" s="37" t="s">
-        <v>279</v>
+        <v>261</v>
       </c>
       <c r="K20" s="37" t="s">
-        <v>280</v>
+        <v>262</v>
       </c>
       <c r="L20" s="37" t="s">
         <v>76</v>
       </c>
       <c r="M20" s="37" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="18" thickBot="1">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="H21" s="37" t="s">
-        <v>282</v>
+        <v>264</v>
       </c>
       <c r="I21" s="37">
         <v>120</v>
       </c>
       <c r="J21" s="37" t="s">
-        <v>283</v>
+        <v>265</v>
       </c>
       <c r="K21" s="37" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
       <c r="L21" s="37" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
       <c r="M21" s="37" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="18" thickBot="1">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="H22" s="37" t="s">
-        <v>286</v>
+        <v>268</v>
       </c>
       <c r="I22" s="37">
         <v>1</v>
       </c>
       <c r="J22" s="37" t="s">
-        <v>287</v>
+        <v>269</v>
       </c>
       <c r="K22" s="37" t="s">
-        <v>288</v>
+        <v>270</v>
       </c>
       <c r="L22" s="37" t="s">
         <v>80</v>
       </c>
       <c r="M22" s="37" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="18" thickBot="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="H23" s="37" t="s">
-        <v>290</v>
+        <v>272</v>
       </c>
       <c r="I23" s="37">
         <v>1</v>
       </c>
       <c r="J23" s="37" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="K23" s="40"/>
       <c r="L23" s="37" t="s">
@@ -4857,7 +4900,7 @@
       <selection sqref="A1:F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.90625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.7265625" style="3"/>
@@ -4867,17 +4910,17 @@
     <col min="6" max="6" width="52.26953125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1">
-      <c r="A1" s="66" t="s">
-        <v>219</v>
-      </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-    </row>
-    <row r="2" spans="1:6" ht="35.5" thickBot="1">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="60" t="s">
+        <v>201</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+    </row>
+    <row r="2" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="20" t="s">
         <v>49</v>
       </c>
@@ -4888,16 +4931,16 @@
         <v>51</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="E2" s="20" t="s">
         <v>53</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="18" thickBot="1">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="18" t="s">
         <v>55</v>
       </c>
@@ -4914,10 +4957,10 @@
         <v>58</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="18" thickBot="1">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="21" t="s">
         <v>60</v>
       </c>
@@ -4934,10 +4977,10 @@
         <v>58</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="18" thickBot="1">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="21" t="s">
         <v>64</v>
       </c>
@@ -4954,358 +4997,358 @@
         <v>58</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="18" thickBot="1">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="18" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="B6" s="18">
         <v>2</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>58</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="18" thickBot="1">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="18" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="B7" s="18">
         <v>30</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="E7" s="18" t="s">
         <v>58</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="18" thickBot="1">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="18" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="B8" s="18">
         <v>42</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>233</v>
+        <v>215</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="18" thickBot="1">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="18" t="s">
-        <v>237</v>
+        <v>219</v>
       </c>
       <c r="B9" s="18">
         <v>120</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>238</v>
+        <v>220</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>239</v>
+        <v>221</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="35.5" thickBot="1">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="18" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
       <c r="B10" s="18">
         <v>8</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>242</v>
+        <v>224</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="35.5" thickBot="1">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="18" t="s">
-        <v>245</v>
+        <v>227</v>
       </c>
       <c r="B11" s="18">
         <v>9</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>246</v>
+        <v>228</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>247</v>
+        <v>229</v>
       </c>
       <c r="E11" s="18" t="s">
         <v>58</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="35.5" thickBot="1">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="18" t="s">
-        <v>249</v>
+        <v>231</v>
       </c>
       <c r="B12" s="18">
         <v>9</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>250</v>
+        <v>232</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="E12" s="18" t="s">
         <v>58</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="35.5" thickBot="1">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="18" t="s">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="B13" s="18">
         <v>6</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>254</v>
+        <v>236</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>58</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="35.5" thickBot="1">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="18" t="s">
-        <v>255</v>
+        <v>237</v>
       </c>
       <c r="B14" s="18">
         <v>6</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="E14" s="18" t="s">
         <v>58</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="35.5" thickBot="1">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="18" t="s">
-        <v>258</v>
+        <v>240</v>
       </c>
       <c r="B15" s="18">
         <v>4</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>259</v>
+        <v>241</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="35.5" thickBot="1">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="18" t="s">
-        <v>262</v>
+        <v>244</v>
       </c>
       <c r="B16" s="18">
         <v>4</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>264</v>
+        <v>246</v>
       </c>
       <c r="E16" s="18" t="s">
         <v>58</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="35.5" thickBot="1">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="18" t="s">
-        <v>266</v>
+        <v>248</v>
       </c>
       <c r="B17" s="18">
         <v>5</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>268</v>
+        <v>250</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>58</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="35.5" thickBot="1">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="18" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="B18" s="18">
         <v>5</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>271</v>
+        <v>253</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>272</v>
+        <v>254</v>
       </c>
       <c r="E18" s="18" t="s">
         <v>58</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="35.5" thickBot="1">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="18" t="s">
-        <v>274</v>
+        <v>256</v>
       </c>
       <c r="B19" s="18">
         <v>6</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>275</v>
+        <v>257</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>276</v>
+        <v>258</v>
       </c>
       <c r="E19" s="18" t="s">
         <v>58</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="35.5" thickBot="1">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="18" t="s">
-        <v>278</v>
+        <v>260</v>
       </c>
       <c r="B20" s="18">
         <v>8</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>279</v>
+        <v>261</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>280</v>
+        <v>262</v>
       </c>
       <c r="E20" s="18" t="s">
         <v>76</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="35.5" thickBot="1">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="18" t="s">
-        <v>282</v>
+        <v>264</v>
       </c>
       <c r="B21" s="18">
         <v>120</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>283</v>
+        <v>265</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>284</v>
+        <v>266</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>235</v>
+        <v>217</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="35.5" thickBot="1">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="18" t="s">
-        <v>286</v>
+        <v>268</v>
       </c>
       <c r="B22" s="18">
         <v>1</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>287</v>
+        <v>269</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>288</v>
+        <v>270</v>
       </c>
       <c r="E22" s="18" t="s">
         <v>80</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="35.5" thickBot="1">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="18" t="s">
-        <v>290</v>
+        <v>272</v>
       </c>
       <c r="B23" s="18">
         <v>1</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="D23" s="27"/>
       <c r="E23" s="18" t="s">

</xml_diff>

<commit_message>
Cleanup and preparation to hide test messages creation behind a facade
</commit_message>
<xml_diff>
--- a/test_bl/resources/tests/TrassaTests_v01.xlsx
+++ b/test_bl/resources/tests/TrassaTests_v01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13380" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13380" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="trassa_Tests" sheetId="3" r:id="rId1"/>
@@ -1057,19 +1057,10 @@
     <t>AIVDM type 5 or 24</t>
   </si>
   <si>
-    <t>Field: MMSI</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>Field: IMO Number</t>
-  </si>
-  <si>
     <t>Not available in type 24</t>
-  </si>
-  <si>
-    <t>Field: Call Sign</t>
   </si>
   <si>
     <t>1) Поля из сообщения AIVDM (5,24) должны быть перенесены согласно таблице мапинга  (см. Таблицу  $PAISD; Note: поле IMO Number отсутствует в  AIVDM (24) )
@@ -1387,7 +1378,16 @@
     </r>
   </si>
   <si>
-    <t>Field: Vessel Name</t>
+    <t>AIVDM Field: MMSI</t>
+  </si>
+  <si>
+    <t>AIVDM Field: IMO Number</t>
+  </si>
+  <si>
+    <t>AIVDM Field: Call Sign</t>
+  </si>
+  <si>
+    <t>AIVDM Field: Vessel Name</t>
   </si>
 </sst>
 </file>
@@ -1812,6 +1812,45 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1825,45 +1864,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2363,14 +2363,14 @@
         <v>315</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D5" s="31"/>
       <c r="E5" s="33" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="F5" s="33" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G5" s="33"/>
       <c r="H5" s="34"/>
@@ -2383,14 +2383,14 @@
         <v>315</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D6" s="31"/>
       <c r="E6" s="33" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="F6" s="33" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="G6" s="33"/>
       <c r="H6" s="34"/>
@@ -2429,7 +2429,7 @@
       </c>
       <c r="D8" s="31"/>
       <c r="E8" s="33" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="F8" s="33" t="s">
         <v>323</v>
@@ -2469,7 +2469,7 @@
       </c>
       <c r="D10" s="50"/>
       <c r="E10" s="53" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="F10" s="53" t="s">
         <v>330</v>
@@ -2489,10 +2489,10 @@
       </c>
       <c r="D11" s="50"/>
       <c r="E11" s="53" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="F11" s="53" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="G11" s="53"/>
       <c r="H11" s="54"/>
@@ -2505,14 +2505,14 @@
         <v>316</v>
       </c>
       <c r="C12" s="52" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D12" s="54"/>
       <c r="E12" s="53" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="F12" s="53" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="G12" s="54"/>
       <c r="H12" s="54"/>
@@ -2527,10 +2527,10 @@
       <c r="C13" s="52"/>
       <c r="D13" s="54"/>
       <c r="E13" s="53" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="F13" s="53" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="G13" s="54"/>
       <c r="H13" s="54"/>
@@ -2545,10 +2545,10 @@
       <c r="C14" s="52"/>
       <c r="D14" s="54"/>
       <c r="E14" s="53" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="F14" s="53" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="G14" s="54"/>
       <c r="H14" s="54"/>
@@ -2563,10 +2563,10 @@
       <c r="C15" s="52"/>
       <c r="D15" s="54"/>
       <c r="E15" s="53" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="F15" s="53" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="G15" s="54"/>
       <c r="H15" s="54"/>
@@ -2876,7 +2876,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2889,144 +2889,144 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="43" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="57" t="s">
         <v>138</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="62" t="s">
+      <c r="B1" s="58"/>
+      <c r="C1" s="56" t="s">
         <v>326</v>
       </c>
-      <c r="D1" s="67" t="s">
-        <v>333</v>
+      <c r="D1" s="61" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="4" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="63" t="s">
+        <v>350</v>
+      </c>
+      <c r="B2" s="62" t="s">
+        <v>359</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>369</v>
+      </c>
+      <c r="D2" s="60"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="63" t="s">
+        <v>351</v>
+      </c>
+      <c r="B3" s="62" t="s">
+        <v>360</v>
+      </c>
+      <c r="C3" s="66" t="s">
+        <v>370</v>
+      </c>
+      <c r="D3" s="60"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="64" t="s">
+        <v>352</v>
+      </c>
+      <c r="B4" s="62" t="s">
+        <v>361</v>
+      </c>
+      <c r="C4" s="67" t="s">
+        <v>327</v>
+      </c>
+      <c r="D4" s="60"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="63" t="s">
         <v>353</v>
       </c>
-      <c r="B2" s="68" t="s">
+      <c r="B5" s="62" t="s">
         <v>362</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C5" s="66" t="s">
+        <v>371</v>
+      </c>
+      <c r="D5" s="60"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="63" t="s">
+        <v>354</v>
+      </c>
+      <c r="B6" s="62" t="s">
+        <v>363</v>
+      </c>
+      <c r="C6" s="67" t="s">
+        <v>327</v>
+      </c>
+      <c r="D6" s="60"/>
+    </row>
+    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="63" t="s">
+        <v>355</v>
+      </c>
+      <c r="B7" s="62" t="s">
+        <v>364</v>
+      </c>
+      <c r="C7" s="66" t="s">
         <v>372</v>
       </c>
-      <c r="D2" s="66"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="69" t="s">
-        <v>354</v>
-      </c>
-      <c r="B3" s="68" t="s">
-        <v>363</v>
-      </c>
-      <c r="C3" s="72" t="s">
+      <c r="D7" s="60" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="63" t="s">
+        <v>356</v>
+      </c>
+      <c r="B8" s="62" t="s">
+        <v>365</v>
+      </c>
+      <c r="C8" s="66" t="s">
         <v>373</v>
       </c>
-      <c r="D3" s="66"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="70" t="s">
-        <v>355</v>
-      </c>
-      <c r="B4" s="68" t="s">
-        <v>364</v>
-      </c>
-      <c r="C4" s="73" t="s">
+      <c r="D8" s="60"/>
+    </row>
+    <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="63" t="s">
+        <v>357</v>
+      </c>
+      <c r="B9" s="62" t="s">
+        <v>366</v>
+      </c>
+      <c r="C9" s="66" t="s">
+        <v>374</v>
+      </c>
+      <c r="D9" s="60"/>
+    </row>
+    <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="63" t="s">
+        <v>325</v>
+      </c>
+      <c r="B10" s="62" t="s">
+        <v>367</v>
+      </c>
+      <c r="C10" s="67" t="s">
         <v>327</v>
       </c>
-      <c r="D4" s="66"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="69" t="s">
-        <v>356</v>
-      </c>
-      <c r="B5" s="68" t="s">
-        <v>365</v>
-      </c>
-      <c r="C5" s="72" t="s">
-        <v>374</v>
-      </c>
-      <c r="D5" s="66"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="69" t="s">
-        <v>357</v>
-      </c>
-      <c r="B6" s="68" t="s">
-        <v>366</v>
-      </c>
-      <c r="C6" s="73" t="s">
-        <v>327</v>
-      </c>
-      <c r="D6" s="66"/>
-    </row>
-    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="69" t="s">
+      <c r="D10" s="60"/>
+    </row>
+    <row r="11" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="63" t="s">
         <v>358</v>
       </c>
-      <c r="B7" s="68" t="s">
-        <v>367</v>
-      </c>
-      <c r="C7" s="72" t="s">
-        <v>375</v>
-      </c>
-      <c r="D7" s="66" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="69" t="s">
-        <v>359</v>
-      </c>
-      <c r="B8" s="68" t="s">
+      <c r="B11" s="62" t="s">
         <v>368</v>
       </c>
-      <c r="C8" s="72" t="s">
-        <v>376</v>
-      </c>
-      <c r="D8" s="66"/>
-    </row>
-    <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="69" t="s">
-        <v>360</v>
-      </c>
-      <c r="B9" s="68" t="s">
-        <v>369</v>
-      </c>
-      <c r="C9" s="72" t="s">
-        <v>377</v>
-      </c>
-      <c r="D9" s="66"/>
-    </row>
-    <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="69" t="s">
-        <v>325</v>
-      </c>
-      <c r="B10" s="68" t="s">
-        <v>370</v>
-      </c>
-      <c r="C10" s="73" t="s">
-        <v>327</v>
-      </c>
-      <c r="D10" s="66"/>
-    </row>
-    <row r="11" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="69" t="s">
-        <v>361</v>
-      </c>
-      <c r="B11" s="68" t="s">
-        <v>371</v>
-      </c>
-      <c r="C11" s="61"/>
-      <c r="D11" s="66"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="60"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="71" t="s">
+      <c r="A12" s="65" t="s">
         <v>145</v>
       </c>
-      <c r="B12" s="65"/>
-      <c r="C12" s="61"/>
-      <c r="D12" s="66"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="60"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3039,7 +3039,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="H2" sqref="H2:I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3056,24 +3056,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="55" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="68" t="s">
         <v>151</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
     </row>
     <row r="2" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="70" t="s">
         <v>152</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
       <c r="H2" s="24" t="s">
         <v>153</v>
       </c>
@@ -3526,8 +3526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3541,21 +3541,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="72"/>
     </row>
     <row r="2" spans="1:13" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="20" t="s">
@@ -3985,6 +3985,7 @@
     <hyperlink ref="F22" r:id="rId1" location="IALA" display="http://catb.org/gpsd/AIVDM.html - IALA"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3992,8 +3993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4015,7 +4016,7 @@
         <v>331</v>
       </c>
       <c r="D1" s="49" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -4026,7 +4027,7 @@
         <v>146</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>332</v>
+        <v>375</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="58" x14ac:dyDescent="0.35">
@@ -4037,10 +4038,10 @@
         <v>147</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>334</v>
+        <v>376</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
@@ -4051,7 +4052,7 @@
         <v>148</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>336</v>
+        <v>377</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
@@ -4911,14 +4912,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="73" t="s">
         <v>201</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
     </row>
     <row r="2" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="20" t="s">

</xml_diff>